<commit_message>
AUD STD with 1 future rolling day
</commit_message>
<xml_diff>
--- a/QuantLibXL/Data2/XLS/AUD/AUD_YCSTDBootstrapping.xlsx
+++ b/QuantLibXL/Data2/XLS/AUD/AUD_YCSTDBootstrapping.xlsx
@@ -654,21 +654,21 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <numFmts count="15">
-    <numFmt numFmtId="43" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
-    <numFmt numFmtId="164" formatCode="ddd\,\ d\-mmm\-yyyy"/>
-    <numFmt numFmtId="165" formatCode="0.0000%"/>
-    <numFmt numFmtId="166" formatCode="0.0000"/>
-    <numFmt numFmtId="167" formatCode="0.000000000"/>
-    <numFmt numFmtId="168" formatCode="0.000000"/>
-    <numFmt numFmtId="169" formatCode="ddd\,\ dd\-mmm\-yyyy"/>
-    <numFmt numFmtId="170" formatCode="ddd\,\ dd\-mmm\-yyyy\,\ hh:mm:ss"/>
-    <numFmt numFmtId="171" formatCode="ddd\,\ d\-mmm\-yy"/>
-    <numFmt numFmtId="172" formatCode="ddd\,\ d\-mmm\-yyyy\,\ hh:mm:ss"/>
-    <numFmt numFmtId="173" formatCode="General_)"/>
-    <numFmt numFmtId="174" formatCode="#,##0.0;#,##0.0"/>
-    <numFmt numFmtId="175" formatCode="&quot;£&quot;#,##0;[Red]\-&quot;£&quot;#,##0"/>
-    <numFmt numFmtId="176" formatCode="[$-409]d\-mmm\-yy;@"/>
-    <numFmt numFmtId="177" formatCode="mm/dd/yy;@"/>
+    <numFmt numFmtId="164" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
+    <numFmt numFmtId="165" formatCode="ddd\,\ d\-mmm\-yyyy"/>
+    <numFmt numFmtId="166" formatCode="0.0000%"/>
+    <numFmt numFmtId="167" formatCode="0.0000"/>
+    <numFmt numFmtId="168" formatCode="0.000000000"/>
+    <numFmt numFmtId="169" formatCode="0.000000"/>
+    <numFmt numFmtId="170" formatCode="ddd\,\ dd\-mmm\-yyyy"/>
+    <numFmt numFmtId="171" formatCode="ddd\,\ dd\-mmm\-yyyy\,\ hh:mm:ss"/>
+    <numFmt numFmtId="172" formatCode="ddd\,\ d\-mmm\-yy"/>
+    <numFmt numFmtId="173" formatCode="ddd\,\ d\-mmm\-yyyy\,\ hh:mm:ss"/>
+    <numFmt numFmtId="174" formatCode="General_)"/>
+    <numFmt numFmtId="175" formatCode="#,##0.0;#,##0.0"/>
+    <numFmt numFmtId="176" formatCode="&quot;£&quot;#,##0;[Red]\-&quot;£&quot;#,##0"/>
+    <numFmt numFmtId="177" formatCode="[$-409]d\-mmm\-yy;@"/>
+    <numFmt numFmtId="178" formatCode="mm/dd/yy;@"/>
   </numFmts>
   <fonts count="25" x14ac:knownFonts="1">
     <font>
@@ -1297,13 +1297,13 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
     <xf numFmtId="38" fontId="9" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="40" fontId="9" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="173" fontId="10" fillId="0" borderId="0"/>
-    <xf numFmtId="174" fontId="11" fillId="9" borderId="0">
+    <xf numFmtId="174" fontId="10" fillId="0" borderId="0"/>
+    <xf numFmtId="175" fontId="11" fillId="9" borderId="0">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="175" fontId="9" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="175" fontId="9" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="43" fontId="24" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="176" fontId="9" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="176" fontId="9" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="164" fontId="24" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="24" fillId="0" borderId="0"/>
@@ -1324,16 +1324,16 @@
     <xf numFmtId="0" fontId="2" fillId="2" borderId="4" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="164" fontId="2" fillId="2" borderId="27" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="2" fillId="2" borderId="27" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="167" fontId="2" fillId="2" borderId="5" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="168" fontId="2" fillId="2" borderId="5" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="164" fontId="2" fillId="2" borderId="28" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="2" fillId="2" borderId="28" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="170" fontId="2" fillId="2" borderId="0" xfId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="171" fontId="2" fillId="2" borderId="0" xfId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="6" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1357,7 +1357,7 @@
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="171" fontId="2" fillId="6" borderId="5" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="172" fontId="2" fillId="6" borderId="5" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="5" borderId="28" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1366,14 +1366,14 @@
     <xf numFmtId="1" fontId="5" fillId="4" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="171" fontId="2" fillId="4" borderId="5" xfId="1" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="172" fontId="2" fillId="4" borderId="5" xfId="1" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="5" borderId="26" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="172" fontId="2" fillId="2" borderId="4" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="173" fontId="2" fillId="2" borderId="4" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="5" borderId="27" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -1382,12 +1382,12 @@
     <xf numFmtId="0" fontId="2" fillId="5" borderId="28" xfId="3" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="12" xfId="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="12" fillId="2" borderId="13" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="172" fontId="8" fillId="4" borderId="8" xfId="1" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="173" fontId="8" fillId="4" borderId="8" xfId="1" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="13" fillId="5" borderId="7" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="12" fillId="2" borderId="14" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="172" fontId="8" fillId="4" borderId="8" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="173" fontId="8" fillId="4" borderId="8" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="2" borderId="10" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -1396,7 +1396,7 @@
     <xf numFmtId="15" fontId="8" fillId="2" borderId="13" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="8" fillId="5" borderId="7" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="8" fillId="2" borderId="14" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="172" fontId="8" fillId="4" borderId="8" xfId="1" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="173" fontId="8" fillId="4" borderId="8" xfId="1" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="26" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1407,13 +1407,13 @@
     <xf numFmtId="0" fontId="16" fillId="2" borderId="11" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="16" fillId="2" borderId="12" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="16" fillId="2" borderId="13" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="176" fontId="17" fillId="4" borderId="8" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="177" fontId="17" fillId="4" borderId="8" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="16" fillId="2" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="177" fontId="16" fillId="2" borderId="26" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="178" fontId="16" fillId="2" borderId="26" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="18" fillId="2" borderId="9" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1422,10 +1422,10 @@
     <xf numFmtId="0" fontId="16" fillId="2" borderId="14" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="176" fontId="17" fillId="4" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="177" fontId="17" fillId="4" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="177" fontId="16" fillId="10" borderId="7" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="178" fontId="16" fillId="10" borderId="7" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="18" fillId="2" borderId="3" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1452,7 +1452,7 @@
     <xf numFmtId="0" fontId="16" fillId="2" borderId="14" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="32" xfId="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="14" xfId="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="169" fontId="2" fillId="2" borderId="27" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="170" fontId="2" fillId="2" borderId="27" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="4" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1467,7 +1467,7 @@
     <xf numFmtId="0" fontId="18" fillId="3" borderId="21" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="167" fontId="16" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="168" fontId="16" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="18" fillId="5" borderId="20" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
@@ -1477,10 +1477,10 @@
     <xf numFmtId="0" fontId="16" fillId="2" borderId="14" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="165" fontId="16" fillId="2" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="166" fontId="16" fillId="2" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="168" fontId="16" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="169" fontId="16" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="18" fillId="5" borderId="18" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
@@ -1490,30 +1490,30 @@
     <xf numFmtId="0" fontId="16" fillId="2" borderId="12" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="165" fontId="16" fillId="2" borderId="11" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="166" fontId="16" fillId="2" borderId="11" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="169" fontId="16" fillId="2" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="170" fontId="16" fillId="2" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="169" fontId="16" fillId="2" borderId="13" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="170" fontId="16" fillId="2" borderId="13" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="169" fontId="16" fillId="2" borderId="11" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="170" fontId="16" fillId="2" borderId="11" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="169" fontId="16" fillId="2" borderId="10" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="170" fontId="16" fillId="2" borderId="10" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="11" borderId="13" xfId="3" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="169" fontId="2" fillId="2" borderId="26" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="170" fontId="2" fillId="2" borderId="26" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="11" borderId="14" xfId="3" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="169" fontId="2" fillId="2" borderId="6" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="170" fontId="2" fillId="2" borderId="6" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="11" borderId="0" xfId="3" applyFont="1" applyFill="1"/>
@@ -1546,50 +1546,50 @@
     <xf numFmtId="0" fontId="16" fillId="2" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="165" fontId="16" fillId="2" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="166" fontId="16" fillId="2" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="164" fontId="16" fillId="2" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="16" fillId="2" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="164" fontId="16" fillId="2" borderId="4" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="16" fillId="2" borderId="4" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="16" fillId="2" borderId="2" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="165" fontId="16" fillId="2" borderId="2" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="166" fontId="16" fillId="2" borderId="2" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="16" fillId="2" borderId="2" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="164" fontId="16" fillId="2" borderId="2" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="16" fillId="2" borderId="2" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="164" fontId="16" fillId="2" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="16" fillId="2" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="166" fontId="16" fillId="2" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="167" fontId="16" fillId="2" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="10" fontId="15" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="16" fillId="2" borderId="6" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="165" fontId="16" fillId="2" borderId="6" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="166" fontId="16" fillId="2" borderId="6" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="16" fillId="2" borderId="6" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="164" fontId="16" fillId="2" borderId="6" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="16" fillId="2" borderId="6" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="164" fontId="16" fillId="2" borderId="5" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="16" fillId="2" borderId="5" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="165" fontId="16" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="166" fontId="16" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="18" fillId="2" borderId="9" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -1611,11 +1611,11 @@
     <xf numFmtId="0" fontId="16" fillId="2" borderId="3" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="176" fontId="15" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="177" fontId="15" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="16" fillId="2" borderId="7" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="177" fontId="16" fillId="2" borderId="7" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="178" fontId="16" fillId="2" borderId="7" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="22" fillId="2" borderId="12" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -1628,13 +1628,13 @@
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="23" fillId="2" borderId="13" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="176" fontId="17" fillId="4" borderId="7" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="177" fontId="17" fillId="4" borderId="7" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="16" fillId="2" borderId="7" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="165" fontId="16" fillId="2" borderId="7" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="166" fontId="16" fillId="2" borderId="7" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="16" fillId="2" borderId="7" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="16" fillId="2" borderId="26" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="16" fillId="2" borderId="10" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1652,7 +1652,7 @@
     <xf numFmtId="0" fontId="18" fillId="2" borderId="11" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="177" fontId="16" fillId="2" borderId="11" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="178" fontId="16" fillId="2" borderId="11" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="16" fillId="2" borderId="11" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1664,7 +1664,7 @@
     <xf numFmtId="0" fontId="16" fillId="13" borderId="7" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="165" fontId="16" fillId="13" borderId="7" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="166" fontId="16" fillId="13" borderId="7" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="16" fillId="13" borderId="7" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="16" fillId="13" borderId="7" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="16" fillId="13" borderId="26" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1673,7 +1673,7 @@
     <xf numFmtId="0" fontId="16" fillId="13" borderId="26" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="16" fillId="13" borderId="7" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="16" fillId="12" borderId="7" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="166" fontId="16" fillId="2" borderId="6" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="167" fontId="16" fillId="2" borderId="6" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="28" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -2097,7 +2097,7 @@
     <row r="1" spans="1:31" s="3" customFormat="1" ht="12" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B1" s="3" t="str">
         <f>_xll.qlxlVersion(TRUE,Trigger)</f>
-        <v>QuantLibXL 1.6.0 - MS VC++ (version unknown) - Multithreaded Dynamic Runtime library - Release Configuration - May  8 2015 11:10:23</v>
+        <v>QuantLibXL 1.6.0 - MS VC++ (version unknown) - Multithreaded Dynamic Runtime library - Release Configuration - May 13 2015 18:26:25</v>
       </c>
     </row>
     <row r="2" spans="1:31" s="3" customFormat="1" ht="19.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -2426,9 +2426,7 @@
       <c r="C11" s="25" t="s">
         <v>66</v>
       </c>
-      <c r="D11" s="24">
-        <v>42135.705277777779</v>
-      </c>
+      <c r="D11" s="24"/>
       <c r="E11" s="4"/>
       <c r="F11" s="4"/>
       <c r="G11" s="27"/>
@@ -2547,7 +2545,7 @@
       </c>
       <c r="D14" s="21" t="str">
         <f>_xll.qlPiecewiseYieldCurve(D16,NDays,Calendar,_xll.ohPack(Selected!D2:D126),,,,Accuracy,TraitsID,InterpolatorID,Permanent,,ObjectOverwrite)</f>
-        <v>_AUDYCSTD#0021</v>
+        <v>_AUDYCSTD#0002</v>
       </c>
       <c r="E14" s="4"/>
       <c r="F14" s="4"/>
@@ -2883,11 +2881,11 @@
       <c r="B23" s="5"/>
       <c r="C23" s="9">
         <f>_xll.qlTermStructureReferenceDate(YieldCurve)</f>
-        <v>42135</v>
+        <v>42138</v>
       </c>
       <c r="D23" s="8">
         <f>MAX(_xll.ohPack(Selected!J1:J126))</f>
-        <v>3.6232381509052253E-2</v>
+        <v>3.8196471968635168E-2</v>
       </c>
       <c r="E23" s="4"/>
       <c r="F23" s="4"/>
@@ -2922,11 +2920,11 @@
       <c r="B24" s="5"/>
       <c r="C24" s="7">
         <f>MAX(_xll.ohPack(Selected!I2:I126))</f>
-        <v>53094</v>
+        <v>53097</v>
       </c>
       <c r="D24" s="6">
         <f>MIN(_xll.ohPack(Selected!J1:J126))</f>
-        <v>2.058200022462572E-2</v>
+        <v>1.9999452074821584E-2</v>
       </c>
       <c r="E24" s="4"/>
       <c r="F24" s="4"/>
@@ -4382,7 +4380,7 @@
     <row r="2" spans="1:11" ht="11.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="106" t="str">
         <f>Deposits!J3</f>
-        <v>obj_00267#0002</v>
+        <v>obj_002c0#0001</v>
       </c>
       <c r="B2" s="106" t="str">
         <f>SUBSTITUTE(SUBSTITUTE(_xll.qlRateHelperQuoteName(A2),"LastFixing","D"),"Libor","")</f>
@@ -4404,11 +4402,11 @@
       </c>
       <c r="H2" s="108">
         <f>_xll.qlRateHelperEarliestDate($A2,Trigger)</f>
-        <v>42135</v>
+        <v>42138</v>
       </c>
       <c r="I2" s="109">
         <f>_xll.qlRateHelperLatestDate($A2,Trigger)</f>
-        <v>42136</v>
+        <v>42139</v>
       </c>
       <c r="J2" s="60">
         <v>10</v>
@@ -4420,7 +4418,7 @@
     <row r="3" spans="1:11" ht="11.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="106" t="str">
         <f>Deposits!J4</f>
-        <v>obj_0024e#0002</v>
+        <v>obj_00288#0001</v>
       </c>
       <c r="B3" s="106" t="str">
         <f>SUBSTITUTE(SUBSTITUTE(_xll.qlRateHelperQuoteName(A3),"LastFixing","D"),"Libor","")</f>
@@ -4428,7 +4426,7 @@
       </c>
       <c r="C3" s="107">
         <f>_xll.qlRateHelperQuoteValue($A3,Trigger)</f>
-        <v>2.0499999999999997E-2</v>
+        <v>0.02</v>
       </c>
       <c r="D3" s="107"/>
       <c r="E3" s="62" t="b">
@@ -4442,18 +4440,18 @@
       </c>
       <c r="H3" s="108">
         <f>_xll.qlRateHelperEarliestDate($A3,Trigger)</f>
-        <v>42135</v>
+        <v>42138</v>
       </c>
       <c r="I3" s="109">
         <f>_xll.qlRateHelperLatestDate($A3,Trigger)</f>
-        <v>42136</v>
+        <v>42139</v>
       </c>
       <c r="J3" s="60"/>
     </row>
     <row r="4" spans="1:11" ht="11.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="106" t="str">
         <f>Deposits!J5</f>
-        <v>obj_0024d#0003</v>
+        <v>obj_00287#0001</v>
       </c>
       <c r="B4" s="106" t="str">
         <f>SUBSTITUTE(SUBSTITUTE(_xll.qlRateHelperQuoteName(A4),"LastFixing","D"),"Libor","")</f>
@@ -4461,7 +4459,7 @@
       </c>
       <c r="C4" s="107">
         <f>_xll.qlRateHelperQuoteValue($A4,Trigger)</f>
-        <v>2.1749999999999999E-2</v>
+        <v>0.02</v>
       </c>
       <c r="D4" s="107"/>
       <c r="E4" s="62" t="b">
@@ -4475,18 +4473,18 @@
       </c>
       <c r="H4" s="108">
         <f>_xll.qlRateHelperEarliestDate($A4,Trigger)</f>
-        <v>42135</v>
+        <v>42138</v>
       </c>
       <c r="I4" s="109">
         <f>_xll.qlRateHelperLatestDate($A4,Trigger)</f>
-        <v>42136</v>
+        <v>42139</v>
       </c>
       <c r="J4" s="60"/>
     </row>
     <row r="5" spans="1:11" ht="11.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="106" t="str">
         <f>Deposits!J6</f>
-        <v>obj_00255#0002</v>
+        <v>obj_00294#0001</v>
       </c>
       <c r="B5" s="106" t="str">
         <f>SUBSTITUTE(SUBSTITUTE(_xll.qlRateHelperQuoteName(A5),"LastFixing","D"),"Libor","")</f>
@@ -4494,7 +4492,7 @@
       </c>
       <c r="C5" s="107">
         <f>_xll.qlRateHelperQuoteValue($A5,Trigger)</f>
-        <v>2.2000000000000002E-2</v>
+        <v>2.1500000000000005E-2</v>
       </c>
       <c r="D5" s="107"/>
       <c r="E5" s="62" t="b">
@@ -4508,11 +4506,11 @@
       </c>
       <c r="H5" s="108">
         <f>_xll.qlRateHelperEarliestDate($A5,Trigger)</f>
-        <v>42135</v>
+        <v>42138</v>
       </c>
       <c r="I5" s="109">
         <f>_xll.qlRateHelperLatestDate($A5,Trigger)</f>
-        <v>42142</v>
+        <v>42145</v>
       </c>
       <c r="J5" s="60">
         <v>60</v>
@@ -4524,7 +4522,7 @@
     <row r="6" spans="1:11" ht="11.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="106" t="str">
         <f>Deposits!J7</f>
-        <v>obj_00262#0002</v>
+        <v>obj_002c8#0001</v>
       </c>
       <c r="B6" s="106" t="str">
         <f>SUBSTITUTE(SUBSTITUTE(_xll.qlRateHelperQuoteName(A6),"LastFixing","D"),"Libor","")</f>
@@ -4546,17 +4544,17 @@
       </c>
       <c r="H6" s="108">
         <f>_xll.qlRateHelperEarliestDate($A6,Trigger)</f>
-        <v>42135</v>
+        <v>42138</v>
       </c>
       <c r="I6" s="109">
         <f>_xll.qlRateHelperLatestDate($A6,Trigger)</f>
-        <v>42149</v>
+        <v>42152</v>
       </c>
     </row>
     <row r="7" spans="1:11" ht="11.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="106" t="str">
         <f>Deposits!J8</f>
-        <v>obj_00266#0002</v>
+        <v>obj_002cd#0001</v>
       </c>
       <c r="B7" s="106" t="str">
         <f>SUBSTITUTE(SUBSTITUTE(_xll.qlRateHelperQuoteName(A7),"LastFixing","D"),"Libor","")</f>
@@ -4578,17 +4576,17 @@
       </c>
       <c r="H7" s="108">
         <f>_xll.qlRateHelperEarliestDate($A7,Trigger)</f>
-        <v>42135</v>
+        <v>42138</v>
       </c>
       <c r="I7" s="109">
         <f>_xll.qlRateHelperLatestDate($A7,Trigger)</f>
-        <v>42156</v>
+        <v>42159</v>
       </c>
     </row>
     <row r="8" spans="1:11" ht="11.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="106" t="str">
         <f>Deposits!J9</f>
-        <v>obj_00263#0002</v>
+        <v>obj_002cc#0001</v>
       </c>
       <c r="B8" s="106" t="str">
         <f>SUBSTITUTE(SUBSTITUTE(_xll.qlRateHelperQuoteName(A8),"LastFixing","D"),"Libor","")</f>
@@ -4610,17 +4608,17 @@
       </c>
       <c r="H8" s="108">
         <f>_xll.qlRateHelperEarliestDate($A8,Trigger)</f>
-        <v>42135</v>
+        <v>42138</v>
       </c>
       <c r="I8" s="109">
         <f>_xll.qlRateHelperLatestDate($A8,Trigger)</f>
-        <v>42166</v>
+        <v>42170</v>
       </c>
     </row>
     <row r="9" spans="1:11" ht="11.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="106" t="str">
         <f>Deposits!J10</f>
-        <v>obj_00265#0002</v>
+        <v>obj_002c9#0001</v>
       </c>
       <c r="B9" s="106" t="str">
         <f>SUBSTITUTE(SUBSTITUTE(_xll.qlRateHelperQuoteName(A9),"LastFixing","D"),"Libor","")</f>
@@ -4628,7 +4626,7 @@
       </c>
       <c r="C9" s="107">
         <f>_xll.qlRateHelperQuoteValue($A9,Trigger)</f>
-        <v>2.12E-2</v>
+        <v>2.1250000000000002E-2</v>
       </c>
       <c r="D9" s="107"/>
       <c r="E9" s="62" t="b">
@@ -4642,17 +4640,17 @@
       </c>
       <c r="H9" s="108">
         <f>_xll.qlRateHelperEarliestDate($A9,Trigger)</f>
-        <v>42135</v>
+        <v>42138</v>
       </c>
       <c r="I9" s="109">
         <f>_xll.qlRateHelperLatestDate($A9,Trigger)</f>
-        <v>42198</v>
+        <v>42199</v>
       </c>
     </row>
     <row r="10" spans="1:11" ht="11.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="106" t="str">
         <f>Deposits!J11</f>
-        <v>obj_0026e#0002</v>
+        <v>obj_002c7#0001</v>
       </c>
       <c r="B10" s="106" t="str">
         <f>SUBSTITUTE(SUBSTITUTE(_xll.qlRateHelperQuoteName(A10),"LastFixing","D"),"Libor","")</f>
@@ -4660,7 +4658,7 @@
       </c>
       <c r="C10" s="107">
         <f>_xll.qlRateHelperQuoteValue($A10,Trigger)</f>
-        <v>2.1400000000000002E-2</v>
+        <v>2.1450000000000004E-2</v>
       </c>
       <c r="D10" s="107"/>
       <c r="E10" s="62" t="b">
@@ -4674,17 +4672,17 @@
       </c>
       <c r="H10" s="108">
         <f>_xll.qlRateHelperEarliestDate($A10,Trigger)</f>
-        <v>42135</v>
+        <v>42138</v>
       </c>
       <c r="I10" s="109">
         <f>_xll.qlRateHelperLatestDate($A10,Trigger)</f>
-        <v>42227</v>
+        <v>42230</v>
       </c>
     </row>
     <row r="11" spans="1:11" ht="11.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="106" t="str">
         <f>Deposits!J12</f>
-        <v>obj_0026b#0002</v>
+        <v>obj_002c1#0001</v>
       </c>
       <c r="B11" s="106" t="str">
         <f>SUBSTITUTE(SUBSTITUTE(_xll.qlRateHelperQuoteName(A11),"LastFixing","D"),"Libor","")</f>
@@ -4692,7 +4690,7 @@
       </c>
       <c r="C11" s="107">
         <f>_xll.qlRateHelperQuoteValue($A11,Trigger)</f>
-        <v>2.1850000000000005E-2</v>
+        <v>2.1950000000000004E-2</v>
       </c>
       <c r="D11" s="107"/>
       <c r="E11" s="62" t="b">
@@ -4706,17 +4704,17 @@
       </c>
       <c r="H11" s="108">
         <f>_xll.qlRateHelperEarliestDate($A11,Trigger)</f>
-        <v>42135</v>
+        <v>42138</v>
       </c>
       <c r="I11" s="109">
         <f>_xll.qlRateHelperLatestDate($A11,Trigger)</f>
-        <v>42258</v>
+        <v>42261</v>
       </c>
     </row>
     <row r="12" spans="1:11" ht="11.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="106" t="str">
         <f>Deposits!J13</f>
-        <v>obj_0026f#0002</v>
+        <v>obj_002cb#0001</v>
       </c>
       <c r="B12" s="106" t="str">
         <f>SUBSTITUTE(SUBSTITUTE(_xll.qlRateHelperQuoteName(A12),"LastFixing","D"),"Libor","")</f>
@@ -4724,7 +4722,7 @@
       </c>
       <c r="C12" s="107">
         <f>_xll.qlRateHelperQuoteValue($A12,Trigger)</f>
-        <v>2.215E-2</v>
+        <v>2.2250000000000002E-2</v>
       </c>
       <c r="D12" s="107"/>
       <c r="E12" s="62" t="b">
@@ -4738,17 +4736,17 @@
       </c>
       <c r="H12" s="108">
         <f>_xll.qlRateHelperEarliestDate($A12,Trigger)</f>
-        <v>42135</v>
+        <v>42138</v>
       </c>
       <c r="I12" s="109">
         <f>_xll.qlRateHelperLatestDate($A12,Trigger)</f>
-        <v>42289</v>
+        <v>42291</v>
       </c>
     </row>
     <row r="13" spans="1:11" ht="11.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="106" t="str">
         <f>Deposits!J14</f>
-        <v>obj_0026d#0002</v>
+        <v>obj_002c3#0001</v>
       </c>
       <c r="B13" s="106" t="str">
         <f>SUBSTITUTE(SUBSTITUTE(_xll.qlRateHelperQuoteName(A13),"LastFixing","D"),"Libor","")</f>
@@ -4756,7 +4754,7 @@
       </c>
       <c r="C13" s="107">
         <f>_xll.qlRateHelperQuoteValue($A13,Trigger)</f>
-        <v>2.2300000000000004E-2</v>
+        <v>2.2450000000000001E-2</v>
       </c>
       <c r="D13" s="107"/>
       <c r="E13" s="62" t="b">
@@ -4770,17 +4768,17 @@
       </c>
       <c r="H13" s="108">
         <f>_xll.qlRateHelperEarliestDate($A13,Trigger)</f>
-        <v>42135</v>
+        <v>42138</v>
       </c>
       <c r="I13" s="109">
         <f>_xll.qlRateHelperLatestDate($A13,Trigger)</f>
-        <v>42319</v>
+        <v>42324</v>
       </c>
     </row>
     <row r="14" spans="1:11" ht="11.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="106" t="str">
         <f>Deposits!J15</f>
-        <v>obj_00264#0002</v>
+        <v>obj_002c5#0001</v>
       </c>
       <c r="B14" s="106" t="str">
         <f>SUBSTITUTE(SUBSTITUTE(_xll.qlRateHelperQuoteName(A14),"LastFixing","D"),"Libor","")</f>
@@ -4802,17 +4800,17 @@
       </c>
       <c r="H14" s="108">
         <f>_xll.qlRateHelperEarliestDate($A14,Trigger)</f>
-        <v>42135</v>
+        <v>42138</v>
       </c>
       <c r="I14" s="109">
         <f>_xll.qlRateHelperLatestDate($A14,Trigger)</f>
-        <v>42349</v>
+        <v>42352</v>
       </c>
     </row>
     <row r="15" spans="1:11" ht="11.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="106" t="str">
         <f>Deposits!J16</f>
-        <v>obj_00261#0002</v>
+        <v>obj_002c4#0001</v>
       </c>
       <c r="B15" s="106" t="str">
         <f>SUBSTITUTE(SUBSTITUTE(_xll.qlRateHelperQuoteName(A15),"LastFixing","D"),"Libor","")</f>
@@ -4834,17 +4832,17 @@
       </c>
       <c r="H15" s="108">
         <f>_xll.qlRateHelperEarliestDate($A15,Trigger)</f>
-        <v>42135</v>
+        <v>42138</v>
       </c>
       <c r="I15" s="109">
         <f>_xll.qlRateHelperLatestDate($A15,Trigger)</f>
-        <v>42380</v>
+        <v>42383</v>
       </c>
     </row>
     <row r="16" spans="1:11" ht="11.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="106" t="str">
         <f>Deposits!J17</f>
-        <v>obj_00269#0002</v>
+        <v>obj_002ca#0001</v>
       </c>
       <c r="B16" s="106" t="str">
         <f>SUBSTITUTE(SUBSTITUTE(_xll.qlRateHelperQuoteName(A16),"LastFixing","D"),"Libor","")</f>
@@ -4866,17 +4864,17 @@
       </c>
       <c r="H16" s="108">
         <f>_xll.qlRateHelperEarliestDate($A16,Trigger)</f>
-        <v>42135</v>
+        <v>42138</v>
       </c>
       <c r="I16" s="109">
         <f>_xll.qlRateHelperLatestDate($A16,Trigger)</f>
-        <v>42411</v>
+        <v>42415</v>
       </c>
     </row>
     <row r="17" spans="1:9" ht="11.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" s="106" t="str">
         <f>Deposits!J18</f>
-        <v>obj_0026c#0002</v>
+        <v>obj_002c2#0001</v>
       </c>
       <c r="B17" s="106" t="str">
         <f>SUBSTITUTE(SUBSTITUTE(_xll.qlRateHelperQuoteName(A17),"LastFixing","D"),"Libor","")</f>
@@ -4898,17 +4896,17 @@
       </c>
       <c r="H17" s="108">
         <f>_xll.qlRateHelperEarliestDate($A17,Trigger)</f>
-        <v>42135</v>
+        <v>42138</v>
       </c>
       <c r="I17" s="109">
         <f>_xll.qlRateHelperLatestDate($A17,Trigger)</f>
-        <v>42440</v>
+        <v>42443</v>
       </c>
     </row>
     <row r="18" spans="1:9" ht="11.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" s="106" t="str">
         <f>Deposits!J19</f>
-        <v>obj_00268#0002</v>
+        <v>obj_002c6#0001</v>
       </c>
       <c r="B18" s="106" t="str">
         <f>SUBSTITUTE(SUBSTITUTE(_xll.qlRateHelperQuoteName(A18),"LastFixing","D"),"Libor","")</f>
@@ -4930,17 +4928,17 @@
       </c>
       <c r="H18" s="108">
         <f>_xll.qlRateHelperEarliestDate($A18,Trigger)</f>
-        <v>42135</v>
+        <v>42138</v>
       </c>
       <c r="I18" s="109">
         <f>_xll.qlRateHelperLatestDate($A18,Trigger)</f>
-        <v>42471</v>
+        <v>42474</v>
       </c>
     </row>
     <row r="19" spans="1:9" ht="11.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A19" s="106" t="str">
         <f>Deposits!J20</f>
-        <v>obj_0026a#0002</v>
+        <v>obj_002ce#0001</v>
       </c>
       <c r="B19" s="106" t="str">
         <f>SUBSTITUTE(SUBSTITUTE(_xll.qlRateHelperQuoteName(A19),"LastFixing","D"),"Libor","")</f>
@@ -4962,17 +4960,17 @@
       </c>
       <c r="H19" s="108">
         <f>_xll.qlRateHelperEarliestDate($A19,Trigger)</f>
-        <v>42135</v>
+        <v>42138</v>
       </c>
       <c r="I19" s="109">
         <f>_xll.qlRateHelperLatestDate($A19,Trigger)</f>
-        <v>42501</v>
+        <v>42506</v>
       </c>
     </row>
     <row r="20" spans="1:9" ht="11.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A20" s="117" t="str">
         <f>Futures!I5</f>
-        <v>obj_00394#0001</v>
+        <v>obj_0026f#0001</v>
       </c>
       <c r="B20" s="117" t="str">
         <f>SUBSTITUTE(SUBSTITUTE(_xll.qlRateHelperQuoteName(A20),"LastFixing","D"),"Libor","")</f>
@@ -4980,7 +4978,7 @@
       </c>
       <c r="C20" s="162">
         <f>_xll.qlRateHelperQuoteValue(A20,Trigger)</f>
-        <v>97.844999999999999</v>
+        <v>97.835000000000008</v>
       </c>
       <c r="D20" s="118">
         <f>_xll.qlFuturesRateHelperConvexityAdjustment(A20,Trigger)</f>
@@ -5007,7 +5005,7 @@
     <row r="21" spans="1:9" ht="11.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A21" s="106" t="str">
         <f>Futures!I6</f>
-        <v>obj_0038d#0001</v>
+        <v>obj_00274#0001</v>
       </c>
       <c r="B21" s="106" t="str">
         <f>SUBSTITUTE(SUBSTITUTE(_xll.qlRateHelperQuoteName(A21),"LastFixing","D"),"Libor","")</f>
@@ -5042,7 +5040,7 @@
     <row r="22" spans="1:9" ht="11.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A22" s="106" t="str">
         <f>Futures!I7</f>
-        <v>obj_00386#0001</v>
+        <v>obj_00277#0001</v>
       </c>
       <c r="B22" s="106" t="str">
         <f>SUBSTITUTE(SUBSTITUTE(_xll.qlRateHelperQuoteName(A22),"LastFixing","D"),"Libor","")</f>
@@ -5077,7 +5075,7 @@
     <row r="23" spans="1:9" ht="11.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A23" s="106" t="str">
         <f>Futures!I8</f>
-        <v>obj_00385#0001</v>
+        <v>obj_00273#0001</v>
       </c>
       <c r="B23" s="106" t="str">
         <f>SUBSTITUTE(SUBSTITUTE(_xll.qlRateHelperQuoteName(A23),"LastFixing","D"),"Libor","")</f>
@@ -5085,7 +5083,7 @@
       </c>
       <c r="C23" s="115">
         <f>_xll.qlRateHelperQuoteValue(A23,Trigger)</f>
-        <v>97.89500000000001</v>
+        <v>97.884999999999991</v>
       </c>
       <c r="D23" s="107">
         <f>_xll.qlFuturesRateHelperConvexityAdjustment(A23,Trigger)</f>
@@ -5112,7 +5110,7 @@
     <row r="24" spans="1:9" ht="11.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A24" s="106" t="str">
         <f>Futures!I9</f>
-        <v>obj_00388#0001</v>
+        <v>obj_0027f#0001</v>
       </c>
       <c r="B24" s="106" t="str">
         <f>SUBSTITUTE(SUBSTITUTE(_xll.qlRateHelperQuoteName(A24),"LastFixing","D"),"Libor","")</f>
@@ -5147,7 +5145,7 @@
     <row r="25" spans="1:9" ht="11.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A25" s="106" t="str">
         <f>Futures!I10</f>
-        <v>obj_003a3#0001</v>
+        <v>obj_0026b#0001</v>
       </c>
       <c r="B25" s="106" t="str">
         <f>SUBSTITUTE(SUBSTITUTE(_xll.qlRateHelperQuoteName(A25),"LastFixing","D"),"Libor","")</f>
@@ -5182,7 +5180,7 @@
     <row r="26" spans="1:9" ht="11.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A26" s="106" t="str">
         <f>Futures!I11</f>
-        <v>obj_00397#0001</v>
+        <v>obj_00283#0001</v>
       </c>
       <c r="B26" s="106" t="str">
         <f>SUBSTITUTE(SUBSTITUTE(_xll.qlRateHelperQuoteName(A26),"LastFixing","D"),"Libor","")</f>
@@ -5217,7 +5215,7 @@
     <row r="27" spans="1:9" ht="11.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A27" s="106" t="str">
         <f>Futures!I12</f>
-        <v>obj_00393#0001</v>
+        <v>obj_00269#0001</v>
       </c>
       <c r="B27" s="106" t="str">
         <f>SUBSTITUTE(SUBSTITUTE(_xll.qlRateHelperQuoteName(A27),"LastFixing","D"),"Libor","")</f>
@@ -5252,7 +5250,7 @@
     <row r="28" spans="1:9" ht="11.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A28" s="106" t="str">
         <f>Futures!I13</f>
-        <v>obj_00390#0001</v>
+        <v>obj_00284#0001</v>
       </c>
       <c r="B28" s="106" t="str">
         <f>SUBSTITUTE(SUBSTITUTE(_xll.qlRateHelperQuoteName(A28),"LastFixing","D"),"Libor","")</f>
@@ -5287,7 +5285,7 @@
     <row r="29" spans="1:9" ht="11.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A29" s="106" t="str">
         <f>Futures!I14</f>
-        <v>obj_0039f#0001</v>
+        <v>obj_0027d#0001</v>
       </c>
       <c r="B29" s="106" t="str">
         <f>SUBSTITUTE(SUBSTITUTE(_xll.qlRateHelperQuoteName(A29),"LastFixing","D"),"Libor","")</f>
@@ -5295,7 +5293,7 @@
       </c>
       <c r="C29" s="115">
         <f>_xll.qlRateHelperQuoteValue(A29,Trigger)</f>
-        <v>97.844999999999999</v>
+        <v>97.835000000000008</v>
       </c>
       <c r="D29" s="107">
         <f>_xll.qlFuturesRateHelperConvexityAdjustment(A29,Trigger)</f>
@@ -5322,7 +5320,7 @@
     <row r="30" spans="1:9" ht="11.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A30" s="106" t="str">
         <f>Futures!I15</f>
-        <v>obj_00380#0001</v>
+        <v>obj_0027e#0001</v>
       </c>
       <c r="B30" s="106" t="str">
         <f>SUBSTITUTE(SUBSTITUTE(_xll.qlRateHelperQuoteName(A30),"LastFixing","D"),"Libor","")</f>
@@ -5357,7 +5355,7 @@
     <row r="31" spans="1:9" ht="11.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A31" s="106" t="str">
         <f>Futures!I16</f>
-        <v>obj_0037e#0001</v>
+        <v>obj_00281#0001</v>
       </c>
       <c r="B31" s="106" t="str">
         <f>SUBSTITUTE(SUBSTITUTE(_xll.qlRateHelperQuoteName(A31),"LastFixing","D"),"Libor","")</f>
@@ -5392,7 +5390,7 @@
     <row r="32" spans="1:9" ht="11.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A32" s="106" t="str">
         <f>Futures!I17</f>
-        <v>obj_00392#0001</v>
+        <v>obj_00263#0001</v>
       </c>
       <c r="B32" s="106" t="str">
         <f>SUBSTITUTE(SUBSTITUTE(_xll.qlRateHelperQuoteName(A32),"LastFixing","D"),"Libor","")</f>
@@ -5400,7 +5398,7 @@
       </c>
       <c r="C32" s="115">
         <f>_xll.qlRateHelperQuoteValue(A32,Trigger)</f>
-        <v>97.784999999999997</v>
+        <v>97.775000000000006</v>
       </c>
       <c r="D32" s="107">
         <f>_xll.qlFuturesRateHelperConvexityAdjustment(A32,Trigger)</f>
@@ -5427,7 +5425,7 @@
     <row r="33" spans="1:11" ht="11.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A33" s="106" t="str">
         <f>Futures!I18</f>
-        <v>obj_0038f#0001</v>
+        <v>obj_0027c#0001</v>
       </c>
       <c r="B33" s="106" t="str">
         <f>SUBSTITUTE(SUBSTITUTE(_xll.qlRateHelperQuoteName(A33),"LastFixing","D"),"Libor","")</f>
@@ -5435,7 +5433,7 @@
       </c>
       <c r="C33" s="115">
         <f>_xll.qlRateHelperQuoteValue(A33,Trigger)</f>
-        <v>97.715000000000003</v>
+        <v>97.694999999999993</v>
       </c>
       <c r="D33" s="107">
         <f>_xll.qlFuturesRateHelperConvexityAdjustment(A33,Trigger)</f>
@@ -5462,7 +5460,7 @@
     <row r="34" spans="1:11" ht="11.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A34" s="106" t="str">
         <f>Futures!I19</f>
-        <v>obj_0038e#0001</v>
+        <v>obj_00278#0001</v>
       </c>
       <c r="B34" s="106" t="str">
         <f>SUBSTITUTE(SUBSTITUTE(_xll.qlRateHelperQuoteName(A34),"LastFixing","D"),"Libor","")</f>
@@ -5470,7 +5468,7 @@
       </c>
       <c r="C34" s="115">
         <f>_xll.qlRateHelperQuoteValue(A34,Trigger)</f>
-        <v>97.63</v>
+        <v>97.6</v>
       </c>
       <c r="D34" s="107">
         <f>_xll.qlFuturesRateHelperConvexityAdjustment(A34,Trigger)</f>
@@ -5497,7 +5495,7 @@
     <row r="35" spans="1:11" ht="11.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A35" s="106" t="str">
         <f>Futures!I20</f>
-        <v>obj_003a0#0001</v>
+        <v>obj_00285#0001</v>
       </c>
       <c r="B35" s="106" t="str">
         <f>SUBSTITUTE(SUBSTITUTE(_xll.qlRateHelperQuoteName(A35),"LastFixing","D"),"Libor","")</f>
@@ -5505,7 +5503,7 @@
       </c>
       <c r="C35" s="115">
         <f>_xll.qlRateHelperQuoteValue(A35,Trigger)</f>
-        <v>97.545000000000002</v>
+        <v>97.5</v>
       </c>
       <c r="D35" s="107">
         <f>_xll.qlFuturesRateHelperConvexityAdjustment(A35,Trigger)</f>
@@ -5532,7 +5530,7 @@
     <row r="36" spans="1:11" ht="11.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A36" s="106" t="str">
         <f>Futures!I21</f>
-        <v>obj_0039d#0001</v>
+        <v>obj_00276#0001</v>
       </c>
       <c r="B36" s="106" t="str">
         <f>SUBSTITUTE(SUBSTITUTE(_xll.qlRateHelperQuoteName(A36),"LastFixing","D"),"Libor","")</f>
@@ -5540,7 +5538,7 @@
       </c>
       <c r="C36" s="115">
         <f>_xll.qlRateHelperQuoteValue(A36,Trigger)</f>
-        <v>97.454999999999998</v>
+        <v>97.405000000000001</v>
       </c>
       <c r="D36" s="107">
         <f>_xll.qlFuturesRateHelperConvexityAdjustment(A36,Trigger)</f>
@@ -5567,7 +5565,7 @@
     <row r="37" spans="1:11" ht="11.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A37" s="106" t="str">
         <f>Futures!I22</f>
-        <v>obj_00383#0001</v>
+        <v>obj_00267#0001</v>
       </c>
       <c r="B37" s="106" t="str">
         <f>SUBSTITUTE(SUBSTITUTE(_xll.qlRateHelperQuoteName(A37),"LastFixing","D"),"Libor","")</f>
@@ -5575,7 +5573,7 @@
       </c>
       <c r="C37" s="115">
         <f>_xll.qlRateHelperQuoteValue(A37,Trigger)</f>
-        <v>97.37</v>
+        <v>97.32</v>
       </c>
       <c r="D37" s="107">
         <f>_xll.qlFuturesRateHelperConvexityAdjustment(A37,Trigger)</f>
@@ -5602,7 +5600,7 @@
     <row r="38" spans="1:11" ht="11.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A38" s="106" t="str">
         <f>Futures!I23</f>
-        <v>obj_00396#0001</v>
+        <v>obj_00279#0001</v>
       </c>
       <c r="B38" s="106" t="str">
         <f>SUBSTITUTE(SUBSTITUTE(_xll.qlRateHelperQuoteName(A38),"LastFixing","D"),"Libor","")</f>
@@ -5610,7 +5608,7 @@
       </c>
       <c r="C38" s="115">
         <f>_xll.qlRateHelperQuoteValue(A38,Trigger)</f>
-        <v>97.28</v>
+        <v>97.224999999999994</v>
       </c>
       <c r="D38" s="107">
         <f>_xll.qlFuturesRateHelperConvexityAdjustment(A38,Trigger)</f>
@@ -5637,7 +5635,7 @@
     <row r="39" spans="1:11" ht="11.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A39" s="106" t="str">
         <f>Futures!I24</f>
-        <v>obj_0037f#0001</v>
+        <v>obj_00282#0001</v>
       </c>
       <c r="B39" s="106" t="str">
         <f>SUBSTITUTE(SUBSTITUTE(_xll.qlRateHelperQuoteName(A39),"LastFixing","D"),"Libor","")</f>
@@ -5645,7 +5643,7 @@
       </c>
       <c r="C39" s="115">
         <f>_xll.qlRateHelperQuoteValue(A39,Trigger)</f>
-        <v>97.2</v>
+        <v>97.135000000000005</v>
       </c>
       <c r="D39" s="107">
         <f>_xll.qlFuturesRateHelperConvexityAdjustment(A39,Trigger)</f>
@@ -5672,7 +5670,7 @@
     <row r="40" spans="1:11" ht="11.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A40" s="106" t="str">
         <f>Futures!I25</f>
-        <v>obj_0039e#0001</v>
+        <v>obj_0027a#0001</v>
       </c>
       <c r="B40" s="106" t="str">
         <f>SUBSTITUTE(SUBSTITUTE(_xll.qlRateHelperQuoteName(A40),"LastFixing","D"),"Libor","")</f>
@@ -5707,7 +5705,7 @@
     <row r="41" spans="1:11" ht="11.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A41" s="106" t="str">
         <f>Futures!I26</f>
-        <v>obj_0039a#0001</v>
+        <v>obj_00264#0001</v>
       </c>
       <c r="B41" s="106" t="str">
         <f>SUBSTITUTE(SUBSTITUTE(_xll.qlRateHelperQuoteName(A41),"LastFixing","D"),"Libor","")</f>
@@ -5743,7 +5741,7 @@
     <row r="42" spans="1:11" ht="11.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A42" s="106" t="str">
         <f>Futures!I27</f>
-        <v>obj_00382#0001</v>
+        <v>obj_00261#0001</v>
       </c>
       <c r="B42" s="106" t="str">
         <f>SUBSTITUTE(SUBSTITUTE(_xll.qlRateHelperQuoteName(A42),"LastFixing","D"),"Libor","")</f>
@@ -5779,7 +5777,7 @@
     <row r="43" spans="1:11" ht="11.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A43" s="106" t="str">
         <f>Futures!I28</f>
-        <v>obj_00389#0001</v>
+        <v>obj_0025d#0001</v>
       </c>
       <c r="B43" s="106" t="str">
         <f>SUBSTITUTE(SUBSTITUTE(_xll.qlRateHelperQuoteName(A43),"LastFixing","D"),"Libor","")</f>
@@ -5815,7 +5813,7 @@
     <row r="44" spans="1:11" ht="11.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A44" s="106" t="str">
         <f>Futures!I29</f>
-        <v>obj_003a2#0001</v>
+        <v>obj_00265#0001</v>
       </c>
       <c r="B44" s="106" t="str">
         <f>SUBSTITUTE(SUBSTITUTE(_xll.qlRateHelperQuoteName(A44),"LastFixing","D"),"Libor","")</f>
@@ -5851,7 +5849,7 @@
     <row r="45" spans="1:11" ht="11.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A45" s="106" t="str">
         <f>Futures!I30</f>
-        <v>obj_0039c#0001</v>
+        <v>obj_00270#0001</v>
       </c>
       <c r="B45" s="106" t="str">
         <f>SUBSTITUTE(SUBSTITUTE(_xll.qlRateHelperQuoteName(A45),"LastFixing","D"),"Libor","")</f>
@@ -5887,7 +5885,7 @@
     <row r="46" spans="1:11" ht="11.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A46" s="106" t="str">
         <f>Futures!I31</f>
-        <v>obj_0037b#0001</v>
+        <v>obj_00266#0001</v>
       </c>
       <c r="B46" s="106" t="str">
         <f>SUBSTITUTE(SUBSTITUTE(_xll.qlRateHelperQuoteName(A46),"LastFixing","D"),"Libor","")</f>
@@ -5923,7 +5921,7 @@
     <row r="47" spans="1:11" ht="11.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A47" s="106" t="str">
         <f>Futures!I32</f>
-        <v>obj_0038a#0001</v>
+        <v>obj_00262#0001</v>
       </c>
       <c r="B47" s="106" t="str">
         <f>SUBSTITUTE(SUBSTITUTE(_xll.qlRateHelperQuoteName(A47),"LastFixing","D"),"Libor","")</f>
@@ -5959,7 +5957,7 @@
     <row r="48" spans="1:11" ht="11.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A48" s="106" t="str">
         <f>Futures!I33</f>
-        <v>obj_0038c#0001</v>
+        <v>obj_0026e#0001</v>
       </c>
       <c r="B48" s="106" t="str">
         <f>SUBSTITUTE(SUBSTITUTE(_xll.qlRateHelperQuoteName(A48),"LastFixing","D"),"Libor","")</f>
@@ -5995,7 +5993,7 @@
     <row r="49" spans="1:11" ht="11.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A49" s="106" t="str">
         <f>Futures!I34</f>
-        <v>obj_0037d#0001</v>
+        <v>obj_00272#0001</v>
       </c>
       <c r="B49" s="106" t="str">
         <f>SUBSTITUTE(SUBSTITUTE(_xll.qlRateHelperQuoteName(A49),"LastFixing","D"),"Libor","")</f>
@@ -6031,7 +6029,7 @@
     <row r="50" spans="1:11" ht="11.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A50" s="106" t="str">
         <f>Futures!I35</f>
-        <v>obj_00398#0001</v>
+        <v>obj_00280#0001</v>
       </c>
       <c r="B50" s="106" t="str">
         <f>SUBSTITUTE(SUBSTITUTE(_xll.qlRateHelperQuoteName(A50),"LastFixing","D"),"Libor","")</f>
@@ -6067,7 +6065,7 @@
     <row r="51" spans="1:11" ht="11.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A51" s="106" t="str">
         <f>Futures!I36</f>
-        <v>obj_0037c#0001</v>
+        <v>obj_0026c#0001</v>
       </c>
       <c r="B51" s="106" t="str">
         <f>SUBSTITUTE(SUBSTITUTE(_xll.qlRateHelperQuoteName(A51),"LastFixing","D"),"Libor","")</f>
@@ -6103,7 +6101,7 @@
     <row r="52" spans="1:11" ht="11.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A52" s="106" t="str">
         <f>Futures!I37</f>
-        <v>obj_003a4#0001</v>
+        <v>obj_00271#0001</v>
       </c>
       <c r="B52" s="106" t="str">
         <f>SUBSTITUTE(SUBSTITUTE(_xll.qlRateHelperQuoteName(A52),"LastFixing","D"),"Libor","")</f>
@@ -6139,7 +6137,7 @@
     <row r="53" spans="1:11" ht="11.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A53" s="106" t="str">
         <f>Futures!I38</f>
-        <v>obj_00391#0001</v>
+        <v>obj_0025e#0001</v>
       </c>
       <c r="B53" s="106" t="str">
         <f>SUBSTITUTE(SUBSTITUTE(_xll.qlRateHelperQuoteName(A53),"LastFixing","D"),"Libor","")</f>
@@ -6175,7 +6173,7 @@
     <row r="54" spans="1:11" ht="11.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A54" s="106" t="str">
         <f>Futures!I39</f>
-        <v>obj_0038b#0001</v>
+        <v>obj_00268#0001</v>
       </c>
       <c r="B54" s="106" t="str">
         <f>SUBSTITUTE(SUBSTITUTE(_xll.qlRateHelperQuoteName(A54),"LastFixing","D"),"Libor","")</f>
@@ -6211,7 +6209,7 @@
     <row r="55" spans="1:11" ht="11.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A55" s="106" t="str">
         <f>Futures!I40</f>
-        <v>obj_00387#0001</v>
+        <v>obj_0027b#0001</v>
       </c>
       <c r="B55" s="106" t="str">
         <f>SUBSTITUTE(SUBSTITUTE(_xll.qlRateHelperQuoteName(A55),"LastFixing","D"),"Libor","")</f>
@@ -6247,7 +6245,7 @@
     <row r="56" spans="1:11" ht="11.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A56" s="106" t="str">
         <f>Futures!I41</f>
-        <v>obj_0039b#0001</v>
+        <v>obj_0026a#0001</v>
       </c>
       <c r="B56" s="106" t="str">
         <f>SUBSTITUTE(SUBSTITUTE(_xll.qlRateHelperQuoteName(A56),"LastFixing","D"),"Libor","")</f>
@@ -6283,7 +6281,7 @@
     <row r="57" spans="1:11" ht="11.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A57" s="106" t="str">
         <f>Futures!I42</f>
-        <v>obj_00395#0001</v>
+        <v>obj_00275#0001</v>
       </c>
       <c r="B57" s="106" t="str">
         <f>SUBSTITUTE(SUBSTITUTE(_xll.qlRateHelperQuoteName(A57),"LastFixing","D"),"Libor","")</f>
@@ -6319,7 +6317,7 @@
     <row r="58" spans="1:11" ht="11.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A58" s="106" t="str">
         <f>Futures!I43</f>
-        <v>obj_003a1#0001</v>
+        <v>obj_00260#0001</v>
       </c>
       <c r="B58" s="106" t="str">
         <f>SUBSTITUTE(SUBSTITUTE(_xll.qlRateHelperQuoteName(A58),"LastFixing","D"),"Libor","")</f>
@@ -6355,7 +6353,7 @@
     <row r="59" spans="1:11" ht="11.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A59" s="106" t="str">
         <f>Futures!I44</f>
-        <v>obj_00381#0001</v>
+        <v>obj_0025c#0001</v>
       </c>
       <c r="B59" s="106" t="str">
         <f>SUBSTITUTE(SUBSTITUTE(_xll.qlRateHelperQuoteName(A59),"LastFixing","D"),"Libor","")</f>
@@ -6391,7 +6389,7 @@
     <row r="60" spans="1:11" ht="11.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A60" s="106" t="str">
         <f>Futures!I45</f>
-        <v>obj_00384#0001</v>
+        <v>obj_0026d#0001</v>
       </c>
       <c r="B60" s="106" t="str">
         <f>SUBSTITUTE(SUBSTITUTE(_xll.qlRateHelperQuoteName(A60),"LastFixing","D"),"Libor","")</f>
@@ -6427,7 +6425,7 @@
     <row r="61" spans="1:11" ht="11.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A61" s="110" t="str">
         <f>Futures!I46</f>
-        <v>obj_00399#0001</v>
+        <v>obj_0025f#0001</v>
       </c>
       <c r="B61" s="110" t="str">
         <f>SUBSTITUTE(SUBSTITUTE(_xll.qlRateHelperQuoteName(A61),"LastFixing","D"),"Libor","")</f>
@@ -6463,7 +6461,7 @@
     <row r="62" spans="1:11" ht="11.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A62" s="106" t="str">
         <f>Swaps!L6</f>
-        <v>obj_003a5#0015</v>
+        <v>obj_002be#0001</v>
       </c>
       <c r="B62" s="106" t="str">
         <f>SUBSTITUTE(SUBSTITUTE(_xll.qlRateHelperQuoteName(A62),"LastFixing","D"),"Libor","")</f>
@@ -6471,7 +6469,7 @@
       </c>
       <c r="C62" s="118">
         <f>_xll.qlRateHelperQuoteValue($A62,Trigger)</f>
-        <v>2.1150000000000002E-2</v>
+        <v>2.145E-2</v>
       </c>
       <c r="D62" s="118">
         <f>_xll.qlSwapRateHelperSpread($A62,Trigger)</f>
@@ -6488,18 +6486,18 @@
       </c>
       <c r="H62" s="120">
         <f>_xll.qlRateHelperEarliestDate($A62,Trigger)</f>
-        <v>42136</v>
+        <v>42139</v>
       </c>
       <c r="I62" s="121">
         <f>_xll.qlRateHelperLatestDate($A62,Trigger)</f>
-        <v>42502</v>
+        <v>42506</v>
       </c>
       <c r="K62" s="122"/>
     </row>
     <row r="63" spans="1:11" ht="11.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A63" s="106" t="str">
         <f>Swaps!L7</f>
-        <v>obj_003a6#0000</v>
+        <v>obj_002bd#0001</v>
       </c>
       <c r="B63" s="106" t="str">
         <f>SUBSTITUTE(SUBSTITUTE(_xll.qlRateHelperQuoteName(A63),"LastFixing","D"),"Libor","")</f>
@@ -6524,18 +6522,18 @@
       </c>
       <c r="H63" s="108">
         <f>_xll.qlRateHelperEarliestDate($A63,Trigger)</f>
-        <v>42136</v>
+        <v>42139</v>
       </c>
       <c r="I63" s="109">
         <f>_xll.qlRateHelperLatestDate($A63,Trigger)</f>
-        <v>42594</v>
+        <v>42597</v>
       </c>
       <c r="K63" s="122"/>
     </row>
     <row r="64" spans="1:11" ht="11.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A64" s="106" t="str">
         <f>Swaps!L8</f>
-        <v>obj_003a7#0000</v>
+        <v>obj_002bc#0001</v>
       </c>
       <c r="B64" s="106" t="str">
         <f>SUBSTITUTE(SUBSTITUTE(_xll.qlRateHelperQuoteName(A64),"LastFixing","D"),"Libor","")</f>
@@ -6560,18 +6558,18 @@
       </c>
       <c r="H64" s="108">
         <f>_xll.qlRateHelperEarliestDate($A64,Trigger)</f>
-        <v>42136</v>
+        <v>42139</v>
       </c>
       <c r="I64" s="109">
         <f>_xll.qlRateHelperLatestDate($A64,Trigger)</f>
-        <v>42688</v>
+        <v>42689</v>
       </c>
       <c r="K64" s="122"/>
     </row>
     <row r="65" spans="1:11" ht="11.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A65" s="106" t="str">
         <f>Swaps!L9</f>
-        <v>obj_003a8#0000</v>
+        <v>obj_002bb#0001</v>
       </c>
       <c r="B65" s="106" t="str">
         <f>SUBSTITUTE(SUBSTITUTE(_xll.qlRateHelperQuoteName(A65),"LastFixing","D"),"Libor","")</f>
@@ -6596,18 +6594,18 @@
       </c>
       <c r="H65" s="108">
         <f>_xll.qlRateHelperEarliestDate($A65,Trigger)</f>
-        <v>42136</v>
+        <v>42139</v>
       </c>
       <c r="I65" s="109">
         <f>_xll.qlRateHelperLatestDate($A65,Trigger)</f>
-        <v>42779</v>
+        <v>42781</v>
       </c>
       <c r="K65" s="122"/>
     </row>
     <row r="66" spans="1:11" ht="11.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A66" s="106" t="str">
         <f>Swaps!L10</f>
-        <v>obj_003aa#0000</v>
+        <v>obj_002bf#0001</v>
       </c>
       <c r="B66" s="106" t="str">
         <f>SUBSTITUTE(SUBSTITUTE(_xll.qlRateHelperQuoteName(A66),"LastFixing","D"),"Libor","")</f>
@@ -6615,7 +6613,7 @@
       </c>
       <c r="C66" s="107">
         <f>_xll.qlRateHelperQuoteValue($A66,Trigger)</f>
-        <v>2.205E-2</v>
+        <v>2.2599999999999999E-2</v>
       </c>
       <c r="D66" s="107">
         <f>_xll.qlSwapRateHelperSpread($A66,Trigger)</f>
@@ -6632,18 +6630,18 @@
       </c>
       <c r="H66" s="108">
         <f>_xll.qlRateHelperEarliestDate($A66,Trigger)</f>
-        <v>42136</v>
+        <v>42139</v>
       </c>
       <c r="I66" s="109">
         <f>_xll.qlRateHelperLatestDate($A66,Trigger)</f>
-        <v>42867</v>
+        <v>42870</v>
       </c>
       <c r="K66" s="122"/>
     </row>
     <row r="67" spans="1:11" ht="11.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A67" s="106" t="str">
         <f>Swaps!L11</f>
-        <v>obj_003a9#0000</v>
+        <v>obj_002ba#0001</v>
       </c>
       <c r="B67" s="106" t="str">
         <f>SUBSTITUTE(SUBSTITUTE(_xll.qlRateHelperQuoteName(A67),"LastFixing","D"),"Libor","")</f>
@@ -6651,7 +6649,7 @@
       </c>
       <c r="C67" s="107">
         <f>_xll.qlRateHelperQuoteValue($A67,Trigger)</f>
-        <v>2.3300000000000001E-2</v>
+        <v>2.4125000000000004E-2</v>
       </c>
       <c r="D67" s="107">
         <f>_xll.qlSwapRateHelperSpread($A67,Trigger)</f>
@@ -6668,18 +6666,18 @@
       </c>
       <c r="H67" s="108">
         <f>_xll.qlRateHelperEarliestDate($A67,Trigger)</f>
-        <v>42136</v>
+        <v>42139</v>
       </c>
       <c r="I67" s="109">
         <f>_xll.qlRateHelperLatestDate($A67,Trigger)</f>
-        <v>43234</v>
+        <v>43235</v>
       </c>
       <c r="K67" s="122"/>
     </row>
     <row r="68" spans="1:11" ht="11.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A68" s="117" t="str">
         <f>Swaps!L12</f>
-        <v>obj_003ab#0013</v>
+        <v>obj_002aa#0001</v>
       </c>
       <c r="B68" s="117" t="str">
         <f>SUBSTITUTE(SUBSTITUTE(_xll.qlRateHelperQuoteName(A68),"LastFixing","D"),"Libor","")</f>
@@ -6687,7 +6685,7 @@
       </c>
       <c r="C68" s="118">
         <f>_xll.qlRateHelperQuoteValue($A68,Trigger)</f>
-        <v>2.5675E-2</v>
+        <v>2.6699999999999998E-2</v>
       </c>
       <c r="D68" s="118">
         <f>_xll.qlSwapRateHelperSpread($A68,Trigger)</f>
@@ -6704,18 +6702,18 @@
       </c>
       <c r="H68" s="120">
         <f>_xll.qlRateHelperEarliestDate($A68,Trigger)</f>
-        <v>42136</v>
+        <v>42139</v>
       </c>
       <c r="I68" s="121">
         <f>_xll.qlRateHelperLatestDate($A68,Trigger)</f>
-        <v>43598</v>
+        <v>43600</v>
       </c>
       <c r="K68" s="122"/>
     </row>
     <row r="69" spans="1:11" ht="11.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A69" s="106" t="str">
         <f>Swaps!L13</f>
-        <v>obj_003ac#0000</v>
+        <v>obj_002a6#0001</v>
       </c>
       <c r="B69" s="106" t="str">
         <f>SUBSTITUTE(SUBSTITUTE(_xll.qlRateHelperQuoteName(A69),"LastFixing","D"),"Libor","")</f>
@@ -6723,7 +6721,7 @@
       </c>
       <c r="C69" s="107">
         <f>_xll.qlRateHelperQuoteValue($A69,Trigger)</f>
-        <v>2.6974999999999999E-2</v>
+        <v>2.8174999999999999E-2</v>
       </c>
       <c r="D69" s="107">
         <f>_xll.qlSwapRateHelperSpread($A69,Trigger)</f>
@@ -6740,18 +6738,18 @@
       </c>
       <c r="H69" s="108">
         <f>_xll.qlRateHelperEarliestDate($A69,Trigger)</f>
-        <v>42136</v>
+        <v>42139</v>
       </c>
       <c r="I69" s="109">
         <f>_xll.qlRateHelperLatestDate($A69,Trigger)</f>
-        <v>43963</v>
+        <v>43966</v>
       </c>
       <c r="K69" s="122"/>
     </row>
     <row r="70" spans="1:11" ht="11.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A70" s="106" t="str">
         <f>Swaps!L14</f>
-        <v>obj_003b3#0000</v>
+        <v>obj_002a9#0001</v>
       </c>
       <c r="B70" s="106" t="str">
         <f>SUBSTITUTE(SUBSTITUTE(_xll.qlRateHelperQuoteName(A70),"LastFixing","D"),"Libor","")</f>
@@ -6759,7 +6757,7 @@
       </c>
       <c r="C70" s="107">
         <f>_xll.qlRateHelperQuoteValue($A70,Trigger)</f>
-        <v>2.8150000000000005E-2</v>
+        <v>2.9525000000000003E-2</v>
       </c>
       <c r="D70" s="107">
         <f>_xll.qlSwapRateHelperSpread($A70,Trigger)</f>
@@ -6776,18 +6774,18 @@
       </c>
       <c r="H70" s="108">
         <f>_xll.qlRateHelperEarliestDate($A70,Trigger)</f>
-        <v>42136</v>
+        <v>42139</v>
       </c>
       <c r="I70" s="109">
         <f>_xll.qlRateHelperLatestDate($A70,Trigger)</f>
-        <v>44328</v>
+        <v>44333</v>
       </c>
       <c r="K70" s="122"/>
     </row>
     <row r="71" spans="1:11" ht="11.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A71" s="106" t="str">
         <f>Swaps!L15</f>
-        <v>obj_003b9#0000</v>
+        <v>obj_002b0#0001</v>
       </c>
       <c r="B71" s="106" t="str">
         <f>SUBSTITUTE(SUBSTITUTE(_xll.qlRateHelperQuoteName(A71),"LastFixing","D"),"Libor","")</f>
@@ -6795,7 +6793,7 @@
       </c>
       <c r="C71" s="107">
         <f>_xll.qlRateHelperQuoteValue($A71,Trigger)</f>
-        <v>2.92E-2</v>
+        <v>3.0724999999999999E-2</v>
       </c>
       <c r="D71" s="107">
         <f>_xll.qlSwapRateHelperSpread($A71,Trigger)</f>
@@ -6812,18 +6810,18 @@
       </c>
       <c r="H71" s="108">
         <f>_xll.qlRateHelperEarliestDate($A71,Trigger)</f>
-        <v>42136</v>
+        <v>42139</v>
       </c>
       <c r="I71" s="109">
         <f>_xll.qlRateHelperLatestDate($A71,Trigger)</f>
-        <v>44693</v>
+        <v>44697</v>
       </c>
       <c r="K71" s="122"/>
     </row>
     <row r="72" spans="1:11" ht="11.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A72" s="106" t="str">
         <f>Swaps!L16</f>
-        <v>obj_003bb#0000</v>
+        <v>obj_002a8#0001</v>
       </c>
       <c r="B72" s="106" t="str">
         <f>SUBSTITUTE(SUBSTITUTE(_xll.qlRateHelperQuoteName(A72),"LastFixing","D"),"Libor","")</f>
@@ -6831,7 +6829,7 @@
       </c>
       <c r="C72" s="107">
         <f>_xll.qlRateHelperQuoteValue($A72,Trigger)</f>
-        <v>3.0099999999999998E-2</v>
+        <v>3.1800000000000002E-2</v>
       </c>
       <c r="D72" s="107">
         <f>_xll.qlSwapRateHelperSpread($A72,Trigger)</f>
@@ -6848,18 +6846,18 @@
       </c>
       <c r="H72" s="108">
         <f>_xll.qlRateHelperEarliestDate($A72,Trigger)</f>
-        <v>42136</v>
+        <v>42139</v>
       </c>
       <c r="I72" s="109">
         <f>_xll.qlRateHelperLatestDate($A72,Trigger)</f>
-        <v>45058</v>
+        <v>45061</v>
       </c>
       <c r="K72" s="122"/>
     </row>
     <row r="73" spans="1:11" ht="11.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A73" s="106" t="str">
         <f>Swaps!L17</f>
-        <v>obj_003bd#0000</v>
+        <v>obj_002a1#0001</v>
       </c>
       <c r="B73" s="106" t="str">
         <f>SUBSTITUTE(SUBSTITUTE(_xll.qlRateHelperQuoteName(A73),"LastFixing","D"),"Libor","")</f>
@@ -6867,7 +6865,7 @@
       </c>
       <c r="C73" s="107">
         <f>_xll.qlRateHelperQuoteValue($A73,Trigger)</f>
-        <v>3.0849999999999999E-2</v>
+        <v>3.2625000000000001E-2</v>
       </c>
       <c r="D73" s="107">
         <f>_xll.qlSwapRateHelperSpread($A73,Trigger)</f>
@@ -6884,18 +6882,18 @@
       </c>
       <c r="H73" s="108">
         <f>_xll.qlRateHelperEarliestDate($A73,Trigger)</f>
-        <v>42136</v>
+        <v>42139</v>
       </c>
       <c r="I73" s="109">
         <f>_xll.qlRateHelperLatestDate($A73,Trigger)</f>
-        <v>45425</v>
+        <v>45427</v>
       </c>
       <c r="K73" s="122"/>
     </row>
     <row r="74" spans="1:11" ht="11.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A74" s="106" t="str">
         <f>Swaps!L18</f>
-        <v>obj_003c0#0000</v>
+        <v>obj_002b3#0001</v>
       </c>
       <c r="B74" s="106" t="str">
         <f>SUBSTITUTE(SUBSTITUTE(_xll.qlRateHelperQuoteName(A74),"LastFixing","D"),"Libor","")</f>
@@ -6903,7 +6901,7 @@
       </c>
       <c r="C74" s="107">
         <f>_xll.qlRateHelperQuoteValue($A74,Trigger)</f>
-        <v>3.1574999999999999E-2</v>
+        <v>3.3399999999999999E-2</v>
       </c>
       <c r="D74" s="107">
         <f>_xll.qlSwapRateHelperSpread($A74,Trigger)</f>
@@ -6920,18 +6918,18 @@
       </c>
       <c r="H74" s="108">
         <f>_xll.qlRateHelperEarliestDate($A74,Trigger)</f>
-        <v>42136</v>
+        <v>42139</v>
       </c>
       <c r="I74" s="109">
         <f>_xll.qlRateHelperLatestDate($A74,Trigger)</f>
-        <v>45789</v>
+        <v>45792</v>
       </c>
       <c r="K74" s="122"/>
     </row>
     <row r="75" spans="1:11" ht="11.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A75" s="106" t="str">
         <f>Swaps!L19</f>
-        <v>obj_003c3#0000</v>
+        <v>obj_002a7#0001</v>
       </c>
       <c r="B75" s="106" t="str">
         <f>SUBSTITUTE(SUBSTITUTE(_xll.qlRateHelperQuoteName(A75),"LastFixing","D"),"Libor","")</f>
@@ -6956,18 +6954,18 @@
       </c>
       <c r="H75" s="108">
         <f>_xll.qlRateHelperEarliestDate($A75,Trigger)</f>
-        <v>42136</v>
+        <v>42139</v>
       </c>
       <c r="I75" s="109">
         <f>_xll.qlRateHelperLatestDate($A75,Trigger)</f>
-        <v>46154</v>
+        <v>46157</v>
       </c>
       <c r="K75" s="122"/>
     </row>
     <row r="76" spans="1:11" ht="11.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A76" s="106" t="str">
         <f>Swaps!L20</f>
-        <v>obj_003c6#0000</v>
+        <v>obj_0029b#0001</v>
       </c>
       <c r="B76" s="106" t="str">
         <f>SUBSTITUTE(SUBSTITUTE(_xll.qlRateHelperQuoteName(A76),"LastFixing","D"),"Libor","")</f>
@@ -6975,7 +6973,7 @@
       </c>
       <c r="C76" s="107">
         <f>_xll.qlRateHelperQuoteValue($A76,Trigger)</f>
-        <v>3.2850000000000004E-2</v>
+        <v>3.4750000000000003E-2</v>
       </c>
       <c r="D76" s="107">
         <f>_xll.qlSwapRateHelperSpread($A76,Trigger)</f>
@@ -6992,18 +6990,18 @@
       </c>
       <c r="H76" s="108">
         <f>_xll.qlRateHelperEarliestDate($A76,Trigger)</f>
-        <v>42136</v>
+        <v>42139</v>
       </c>
       <c r="I76" s="109">
         <f>_xll.qlRateHelperLatestDate($A76,Trigger)</f>
-        <v>46519</v>
+        <v>46524</v>
       </c>
       <c r="K76" s="122"/>
     </row>
     <row r="77" spans="1:11" ht="11.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A77" s="106" t="str">
         <f>Swaps!L21</f>
-        <v>obj_003ad#0000</v>
+        <v>obj_002a2#0001</v>
       </c>
       <c r="B77" s="106" t="str">
         <f>SUBSTITUTE(SUBSTITUTE(_xll.qlRateHelperQuoteName(A77),"LastFixing","D"),"Libor","")</f>
@@ -7028,18 +7026,18 @@
       </c>
       <c r="H77" s="108">
         <f>_xll.qlRateHelperEarliestDate($A77,Trigger)</f>
-        <v>42136</v>
+        <v>42139</v>
       </c>
       <c r="I77" s="109">
         <f>_xll.qlRateHelperLatestDate($A77,Trigger)</f>
-        <v>46885</v>
+        <v>46888</v>
       </c>
       <c r="K77" s="122"/>
     </row>
     <row r="78" spans="1:11" ht="11.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A78" s="106" t="str">
         <f>Swaps!L22</f>
-        <v>obj_003b4#0000</v>
+        <v>obj_002a5#0001</v>
       </c>
       <c r="B78" s="106" t="str">
         <f>SUBSTITUTE(SUBSTITUTE(_xll.qlRateHelperQuoteName(A78),"LastFixing","D"),"Libor","")</f>
@@ -7064,18 +7062,18 @@
       </c>
       <c r="H78" s="108">
         <f>_xll.qlRateHelperEarliestDate($A78,Trigger)</f>
-        <v>42136</v>
+        <v>42139</v>
       </c>
       <c r="I78" s="109">
         <f>_xll.qlRateHelperLatestDate($A78,Trigger)</f>
-        <v>47252</v>
+        <v>47253</v>
       </c>
       <c r="K78" s="122"/>
     </row>
     <row r="79" spans="1:11" ht="11.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A79" s="106" t="str">
         <f>Swaps!L23</f>
-        <v>obj_003b0#0000</v>
+        <v>obj_002b5#0001</v>
       </c>
       <c r="B79" s="106" t="str">
         <f>SUBSTITUTE(SUBSTITUTE(_xll.qlRateHelperQuoteName(A79),"LastFixing","D"),"Libor","")</f>
@@ -7083,7 +7081,7 @@
       </c>
       <c r="C79" s="107">
         <f>_xll.qlRateHelperQuoteValue($A79,Trigger)</f>
-        <v>3.4200000000000001E-2</v>
+        <v>3.61E-2</v>
       </c>
       <c r="D79" s="107">
         <f>_xll.qlSwapRateHelperSpread($A79,Trigger)</f>
@@ -7100,17 +7098,17 @@
       </c>
       <c r="H79" s="108">
         <f>_xll.qlRateHelperEarliestDate($A79,Trigger)</f>
-        <v>42136</v>
+        <v>42139</v>
       </c>
       <c r="I79" s="109">
         <f>_xll.qlRateHelperLatestDate($A79,Trigger)</f>
-        <v>47616</v>
+        <v>47618</v>
       </c>
     </row>
     <row r="80" spans="1:11" ht="11.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A80" s="106" t="str">
         <f>Swaps!L24</f>
-        <v>obj_003bc#0000</v>
+        <v>obj_002a4#0001</v>
       </c>
       <c r="B80" s="106" t="str">
         <f>SUBSTITUTE(SUBSTITUTE(_xll.qlRateHelperQuoteName(A80),"LastFixing","D"),"Libor","")</f>
@@ -7135,17 +7133,17 @@
       </c>
       <c r="H80" s="108">
         <f>_xll.qlRateHelperEarliestDate($A80,Trigger)</f>
-        <v>42136</v>
+        <v>42139</v>
       </c>
       <c r="I80" s="109">
         <f>_xll.qlRateHelperLatestDate($A80,Trigger)</f>
-        <v>47980</v>
+        <v>47983</v>
       </c>
     </row>
     <row r="81" spans="1:9" ht="11.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A81" s="106" t="str">
         <f>Swaps!L25</f>
-        <v>obj_003be#0000</v>
+        <v>obj_0029e#0001</v>
       </c>
       <c r="B81" s="106" t="str">
         <f>SUBSTITUTE(SUBSTITUTE(_xll.qlRateHelperQuoteName(A81),"LastFixing","D"),"Libor","")</f>
@@ -7170,17 +7168,17 @@
       </c>
       <c r="H81" s="108">
         <f>_xll.qlRateHelperEarliestDate($A81,Trigger)</f>
-        <v>42136</v>
+        <v>42139</v>
       </c>
       <c r="I81" s="109">
         <f>_xll.qlRateHelperLatestDate($A81,Trigger)</f>
-        <v>48346</v>
+        <v>48351</v>
       </c>
     </row>
     <row r="82" spans="1:9" ht="11.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A82" s="106" t="str">
         <f>Swaps!L26</f>
-        <v>obj_003c1#0000</v>
+        <v>obj_002af#0001</v>
       </c>
       <c r="B82" s="106" t="str">
         <f>SUBSTITUTE(SUBSTITUTE(_xll.qlRateHelperQuoteName(A82),"LastFixing","D"),"Libor","")</f>
@@ -7205,17 +7203,17 @@
       </c>
       <c r="H82" s="108">
         <f>_xll.qlRateHelperEarliestDate($A82,Trigger)</f>
-        <v>42136</v>
+        <v>42139</v>
       </c>
       <c r="I82" s="109">
         <f>_xll.qlRateHelperLatestDate($A82,Trigger)</f>
-        <v>48711</v>
+        <v>48715</v>
       </c>
     </row>
     <row r="83" spans="1:9" ht="11.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A83" s="106" t="str">
         <f>Swaps!L27</f>
-        <v>obj_003c4#0000</v>
+        <v>obj_002a3#0001</v>
       </c>
       <c r="B83" s="106" t="str">
         <f>SUBSTITUTE(SUBSTITUTE(_xll.qlRateHelperQuoteName(A83),"LastFixing","D"),"Libor","")</f>
@@ -7240,17 +7238,17 @@
       </c>
       <c r="H83" s="108">
         <f>_xll.qlRateHelperEarliestDate($A83,Trigger)</f>
-        <v>42136</v>
+        <v>42139</v>
       </c>
       <c r="I83" s="109">
         <f>_xll.qlRateHelperLatestDate($A83,Trigger)</f>
-        <v>49076</v>
+        <v>49079</v>
       </c>
     </row>
     <row r="84" spans="1:9" ht="11.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A84" s="106" t="str">
         <f>Swaps!L28</f>
-        <v>obj_003c7#0000</v>
+        <v>obj_002b6#0001</v>
       </c>
       <c r="B84" s="106" t="str">
         <f>SUBSTITUTE(SUBSTITUTE(_xll.qlRateHelperQuoteName(A84),"LastFixing","D"),"Libor","")</f>
@@ -7258,7 +7256,7 @@
       </c>
       <c r="C84" s="107">
         <f>_xll.qlRateHelperQuoteValue($A84,Trigger)</f>
-        <v>3.5125000000000003E-2</v>
+        <v>3.7025000000000002E-2</v>
       </c>
       <c r="D84" s="107">
         <f>_xll.qlSwapRateHelperSpread($A84,Trigger)</f>
@@ -7275,17 +7273,17 @@
       </c>
       <c r="H84" s="108">
         <f>_xll.qlRateHelperEarliestDate($A84,Trigger)</f>
-        <v>42136</v>
+        <v>42139</v>
       </c>
       <c r="I84" s="109">
         <f>_xll.qlRateHelperLatestDate($A84,Trigger)</f>
-        <v>49443</v>
+        <v>49444</v>
       </c>
     </row>
     <row r="85" spans="1:9" ht="11.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A85" s="106" t="str">
         <f>Swaps!L29</f>
-        <v>obj_003ae#0000</v>
+        <v>obj_0029f#0001</v>
       </c>
       <c r="B85" s="106" t="str">
         <f>SUBSTITUTE(SUBSTITUTE(_xll.qlRateHelperQuoteName(A85),"LastFixing","D"),"Libor","")</f>
@@ -7310,17 +7308,17 @@
       </c>
       <c r="H85" s="108">
         <f>_xll.qlRateHelperEarliestDate($A85,Trigger)</f>
-        <v>42136</v>
+        <v>42139</v>
       </c>
       <c r="I85" s="109">
         <f>_xll.qlRateHelperLatestDate($A85,Trigger)</f>
-        <v>49807</v>
+        <v>49810</v>
       </c>
     </row>
     <row r="86" spans="1:9" ht="11.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A86" s="106" t="str">
         <f>Swaps!L30</f>
-        <v>obj_003b5#0000</v>
+        <v>obj_0029d#0001</v>
       </c>
       <c r="B86" s="106" t="str">
         <f>SUBSTITUTE(SUBSTITUTE(_xll.qlRateHelperQuoteName(A86),"LastFixing","D"),"Libor","")</f>
@@ -7345,17 +7343,17 @@
       </c>
       <c r="H86" s="108">
         <f>_xll.qlRateHelperEarliestDate($A86,Trigger)</f>
-        <v>42136</v>
+        <v>42139</v>
       </c>
       <c r="I86" s="109">
         <f>_xll.qlRateHelperLatestDate($A86,Trigger)</f>
-        <v>50172</v>
+        <v>50175</v>
       </c>
     </row>
     <row r="87" spans="1:9" ht="11.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A87" s="106" t="str">
         <f>Swaps!L31</f>
-        <v>obj_003b7#0000</v>
+        <v>obj_002b8#0001</v>
       </c>
       <c r="B87" s="106" t="str">
         <f>SUBSTITUTE(SUBSTITUTE(_xll.qlRateHelperQuoteName(A87),"LastFixing","D"),"Libor","")</f>
@@ -7380,17 +7378,17 @@
       </c>
       <c r="H87" s="108">
         <f>_xll.qlRateHelperEarliestDate($A87,Trigger)</f>
-        <v>42136</v>
+        <v>42139</v>
       </c>
       <c r="I87" s="109">
         <f>_xll.qlRateHelperLatestDate($A87,Trigger)</f>
-        <v>50537</v>
+        <v>50542</v>
       </c>
     </row>
     <row r="88" spans="1:9" ht="11.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A88" s="106" t="str">
         <f>Swaps!L32</f>
-        <v>obj_003b8#0000</v>
+        <v>obj_002b4#0001</v>
       </c>
       <c r="B88" s="106" t="str">
         <f>SUBSTITUTE(SUBSTITUTE(_xll.qlRateHelperQuoteName(A88),"LastFixing","D"),"Libor","")</f>
@@ -7415,17 +7413,17 @@
       </c>
       <c r="H88" s="108">
         <f>_xll.qlRateHelperEarliestDate($A88,Trigger)</f>
-        <v>42136</v>
+        <v>42139</v>
       </c>
       <c r="I88" s="109">
         <f>_xll.qlRateHelperLatestDate($A88,Trigger)</f>
-        <v>50902</v>
+        <v>50906</v>
       </c>
     </row>
     <row r="89" spans="1:9" ht="11.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A89" s="106" t="str">
         <f>Swaps!L33</f>
-        <v>obj_003b2#0000</v>
+        <v>obj_002ad#0001</v>
       </c>
       <c r="B89" s="106" t="str">
         <f>SUBSTITUTE(SUBSTITUTE(_xll.qlRateHelperQuoteName(A89),"LastFixing","D"),"Libor","")</f>
@@ -7433,7 +7431,7 @@
       </c>
       <c r="C89" s="107">
         <f>_xll.qlRateHelperQuoteValue($A89,Trigger)</f>
-        <v>3.5475000000000007E-2</v>
+        <v>3.7375000000000005E-2</v>
       </c>
       <c r="D89" s="107">
         <f>_xll.qlSwapRateHelperSpread($A89,Trigger)</f>
@@ -7450,17 +7448,17 @@
       </c>
       <c r="H89" s="108">
         <f>_xll.qlRateHelperEarliestDate($A89,Trigger)</f>
-        <v>42136</v>
+        <v>42139</v>
       </c>
       <c r="I89" s="109">
         <f>_xll.qlRateHelperLatestDate($A89,Trigger)</f>
-        <v>51270</v>
+        <v>51271</v>
       </c>
     </row>
     <row r="90" spans="1:9" ht="11.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A90" s="106" t="str">
         <f>Swaps!L34</f>
-        <v>obj_003c2#0000</v>
+        <v>obj_002ab#0001</v>
       </c>
       <c r="B90" s="106" t="str">
         <f>SUBSTITUTE(SUBSTITUTE(_xll.qlRateHelperQuoteName(A90),"LastFixing","D"),"Libor","")</f>
@@ -7485,17 +7483,17 @@
       </c>
       <c r="H90" s="108">
         <f>_xll.qlRateHelperEarliestDate($A90,Trigger)</f>
-        <v>42136</v>
+        <v>42139</v>
       </c>
       <c r="I90" s="109">
         <f>_xll.qlRateHelperLatestDate($A90,Trigger)</f>
-        <v>51634</v>
+        <v>51636</v>
       </c>
     </row>
     <row r="91" spans="1:9" ht="11.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A91" s="106" t="str">
         <f>Swaps!L35</f>
-        <v>obj_003c5#0000</v>
+        <v>obj_002a0#0001</v>
       </c>
       <c r="B91" s="106" t="str">
         <f>SUBSTITUTE(SUBSTITUTE(_xll.qlRateHelperQuoteName(A91),"LastFixing","D"),"Libor","")</f>
@@ -7520,17 +7518,17 @@
       </c>
       <c r="H91" s="108">
         <f>_xll.qlRateHelperEarliestDate($A91,Trigger)</f>
-        <v>42136</v>
+        <v>42139</v>
       </c>
       <c r="I91" s="109">
         <f>_xll.qlRateHelperLatestDate($A91,Trigger)</f>
-        <v>51998</v>
+        <v>52001</v>
       </c>
     </row>
     <row r="92" spans="1:9" ht="11.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A92" s="106" t="str">
         <f>Swaps!L36</f>
-        <v>obj_003c8#0000</v>
+        <v>obj_002b2#0001</v>
       </c>
       <c r="B92" s="106" t="str">
         <f>SUBSTITUTE(SUBSTITUTE(_xll.qlRateHelperQuoteName(A92),"LastFixing","D"),"Libor","")</f>
@@ -7555,17 +7553,17 @@
       </c>
       <c r="H92" s="108">
         <f>_xll.qlRateHelperEarliestDate($A92,Trigger)</f>
-        <v>42136</v>
+        <v>42139</v>
       </c>
       <c r="I92" s="109">
         <f>_xll.qlRateHelperLatestDate($A92,Trigger)</f>
-        <v>52363</v>
+        <v>52366</v>
       </c>
     </row>
     <row r="93" spans="1:9" ht="11.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A93" s="106" t="str">
         <f>Swaps!L37</f>
-        <v>obj_003af#0000</v>
+        <v>obj_002b9#0001</v>
       </c>
       <c r="B93" s="106" t="str">
         <f>SUBSTITUTE(SUBSTITUTE(_xll.qlRateHelperQuoteName(A93),"LastFixing","D"),"Libor","")</f>
@@ -7590,17 +7588,17 @@
       </c>
       <c r="H93" s="108">
         <f>_xll.qlRateHelperEarliestDate($A93,Trigger)</f>
-        <v>42136</v>
+        <v>42139</v>
       </c>
       <c r="I93" s="109">
         <f>_xll.qlRateHelperLatestDate($A93,Trigger)</f>
-        <v>52729</v>
+        <v>52733</v>
       </c>
     </row>
     <row r="94" spans="1:9" ht="11.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A94" s="106" t="str">
         <f>Swaps!L38</f>
-        <v>obj_003b6#0000</v>
+        <v>obj_0029c#0001</v>
       </c>
       <c r="B94" s="106" t="str">
         <f>SUBSTITUTE(SUBSTITUTE(_xll.qlRateHelperQuoteName(A94),"LastFixing","D"),"Libor","")</f>
@@ -7608,7 +7606,7 @@
       </c>
       <c r="C94" s="107">
         <f>_xll.qlRateHelperQuoteValue($A94,Trigger)</f>
-        <v>3.56E-2</v>
+        <v>3.7499999999999999E-2</v>
       </c>
       <c r="D94" s="107">
         <f>_xll.qlSwapRateHelperSpread($A94,Trigger)</f>
@@ -7625,17 +7623,17 @@
       </c>
       <c r="H94" s="108">
         <f>_xll.qlRateHelperEarliestDate($A94,Trigger)</f>
-        <v>42136</v>
+        <v>42139</v>
       </c>
       <c r="I94" s="109">
         <f>_xll.qlRateHelperLatestDate($A94,Trigger)</f>
-        <v>53094</v>
+        <v>53097</v>
       </c>
     </row>
     <row r="95" spans="1:9" ht="11.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A95" s="106" t="str">
         <f>Swaps!L39</f>
-        <v>obj_003b1#0000</v>
+        <v>obj_002b1#0001</v>
       </c>
       <c r="B95" s="106" t="str">
         <f>SUBSTITUTE(SUBSTITUTE(_xll.qlRateHelperQuoteName(A95),"LastFixing","D"),"Libor","")</f>
@@ -7660,17 +7658,17 @@
       </c>
       <c r="H95" s="108">
         <f>_xll.qlRateHelperEarliestDate($A95,Trigger)</f>
-        <v>42136</v>
+        <v>42139</v>
       </c>
       <c r="I95" s="109">
         <f>_xll.qlRateHelperLatestDate($A95,Trigger)</f>
-        <v>54920</v>
+        <v>54924</v>
       </c>
     </row>
     <row r="96" spans="1:9" ht="11.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A96" s="106" t="str">
         <f>Swaps!L40</f>
-        <v>obj_003ba#0000</v>
+        <v>obj_002ac#0001</v>
       </c>
       <c r="B96" s="106" t="str">
         <f>SUBSTITUTE(SUBSTITUTE(_xll.qlRateHelperQuoteName(A96),"LastFixing","D"),"Libor","")</f>
@@ -7678,7 +7676,7 @@
       </c>
       <c r="C96" s="107">
         <f>_xll.qlRateHelperQuoteValue($A96,Trigger)</f>
-        <v>3.5000000000000003E-2</v>
+        <v>3.6900000000000002E-2</v>
       </c>
       <c r="D96" s="107">
         <f>_xll.qlSwapRateHelperSpread($A96,Trigger)</f>
@@ -7695,17 +7693,17 @@
       </c>
       <c r="H96" s="108">
         <f>_xll.qlRateHelperEarliestDate($A96,Trigger)</f>
-        <v>42136</v>
+        <v>42139</v>
       </c>
       <c r="I96" s="109">
         <f>_xll.qlRateHelperLatestDate($A96,Trigger)</f>
-        <v>56746</v>
+        <v>56751</v>
       </c>
     </row>
     <row r="97" spans="1:9" ht="11.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A97" s="106" t="str">
         <f>Swaps!L41</f>
-        <v>obj_003bf#0000</v>
+        <v>obj_002b7#0001</v>
       </c>
       <c r="B97" s="106" t="str">
         <f>SUBSTITUTE(SUBSTITUTE(_xll.qlRateHelperQuoteName(A97),"LastFixing","D"),"Libor","")</f>
@@ -7730,17 +7728,17 @@
       </c>
       <c r="H97" s="108">
         <f>_xll.qlRateHelperEarliestDate($A97,Trigger)</f>
-        <v>42136</v>
+        <v>42139</v>
       </c>
       <c r="I97" s="109">
         <f>_xll.qlRateHelperLatestDate($A97,Trigger)</f>
-        <v>60399</v>
+        <v>60402</v>
       </c>
     </row>
     <row r="98" spans="1:9" ht="11.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A98" s="106" t="str">
         <f>Swaps!L42</f>
-        <v>obj_003c9#0000</v>
+        <v>obj_002ae#0001</v>
       </c>
       <c r="B98" s="106" t="str">
         <f>SUBSTITUTE(SUBSTITUTE(_xll.qlRateHelperQuoteName(A98),"LastFixing","D"),"Libor","")</f>
@@ -7765,11 +7763,11 @@
       </c>
       <c r="H98" s="113">
         <f>_xll.qlRateHelperEarliestDate($A98,Trigger)</f>
-        <v>42136</v>
+        <v>42139</v>
       </c>
       <c r="I98" s="114">
         <f>_xll.qlRateHelperLatestDate($A98,Trigger)</f>
-        <v>64052</v>
+        <v>64054</v>
       </c>
     </row>
     <row r="99" spans="1:9" x14ac:dyDescent="0.25">
@@ -7831,7 +7829,7 @@
       </c>
       <c r="J1" s="72">
         <f t="array" ref="J1:J126">_xll.qlPiecewiseYieldCurveData(YieldCurve)</f>
-        <v>2.1749351994906171E-2</v>
+        <v>1.9999452074821584E-2</v>
       </c>
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.2">
@@ -7843,7 +7841,7 @@
       </c>
       <c r="D2" s="75" t="str">
         <f t="array" ref="D2:D126">_xll.qlRateHelperSelection(_xll.ohFilter(RateHelpers,RateHelpersIncluded),_xll.ohFilter(RateHelpersPriority,RateHelpersIncluded),nIMMFutures,nSerialFutures,FrontFuturesRollingDays,DepoInclusionCriteria,_xll.ohFilter(MinDistance,RateHelpersIncluded),Trigger)</f>
-        <v>obj_0024d</v>
+        <v>obj_00287</v>
       </c>
       <c r="E2" s="75" t="str">
         <f>SUBSTITUTE(SUBSTITUTE(_xll.qlRateHelperQuoteName(D2),"LastFixing","D"),"Libor","")</f>
@@ -7851,7 +7849,7 @@
       </c>
       <c r="F2" s="76">
         <f>_xll.qlRateHelperRate($D2)</f>
-        <v>2.1749999999999999E-2</v>
+        <v>0.02</v>
       </c>
       <c r="G2" s="76">
         <f>IF(ISERROR(_xll.qlSwapRateHelperSpread($D2)),IF(ISERROR(_xll.qlFuturesRateHelperConvexityAdjustment($D2)),0,_xll.qlFuturesRateHelperConvexityAdjustment($D2)),_xll.qlSwapRateHelperSpread($D2))</f>
@@ -7859,14 +7857,14 @@
       </c>
       <c r="H2" s="83">
         <f>_xll.qlRateHelperEarliestDate($D2)</f>
-        <v>42135</v>
+        <v>42138</v>
       </c>
       <c r="I2" s="84">
         <f>_xll.qlRateHelperLatestDate($D2)</f>
-        <v>42136</v>
+        <v>42139</v>
       </c>
       <c r="J2" s="72">
-        <v>2.1749351994906171E-2</v>
+        <v>1.9999452074821584E-2</v>
       </c>
       <c r="K2" s="77"/>
     </row>
@@ -7878,7 +7876,7 @@
         <v>0</v>
       </c>
       <c r="D3" s="75" t="str">
-        <v>obj_00255</v>
+        <v>obj_00294</v>
       </c>
       <c r="E3" s="75" t="str">
         <f>SUBSTITUTE(SUBSTITUTE(_xll.qlRateHelperQuoteName(D3),"LastFixing","D"),"Libor","")</f>
@@ -7886,7 +7884,7 @@
       </c>
       <c r="F3" s="76">
         <f>_xll.qlRateHelperRate($D3)</f>
-        <v>2.2000000000000002E-2</v>
+        <v>2.1500000000000005E-2</v>
       </c>
       <c r="G3" s="76">
         <f>IF(ISERROR(_xll.qlSwapRateHelperSpread($D3)),IF(ISERROR(_xll.qlFuturesRateHelperConvexityAdjustment($D3)),0,_xll.qlFuturesRateHelperConvexityAdjustment($D3)),_xll.qlSwapRateHelperSpread($D3))</f>
@@ -7894,14 +7892,14 @@
       </c>
       <c r="H3" s="83">
         <f>_xll.qlRateHelperEarliestDate($D3)</f>
-        <v>42135</v>
+        <v>42138</v>
       </c>
       <c r="I3" s="84">
         <f>_xll.qlRateHelperLatestDate($D3)</f>
-        <v>42142</v>
+        <v>42145</v>
       </c>
       <c r="J3" s="72">
-        <v>2.1995360209201915E-2</v>
+        <v>2.1495568683819147E-2</v>
       </c>
       <c r="K3" s="77"/>
     </row>
@@ -7910,10 +7908,10 @@
         <v>50</v>
       </c>
       <c r="B4" s="79">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D4" s="75" t="str">
-        <v>obj_00262</v>
+        <v>obj_002c8</v>
       </c>
       <c r="E4" s="75" t="str">
         <f>SUBSTITUTE(SUBSTITUTE(_xll.qlRateHelperQuoteName(D4),"LastFixing","D"),"Libor","")</f>
@@ -7929,14 +7927,14 @@
       </c>
       <c r="H4" s="83">
         <f>_xll.qlRateHelperEarliestDate($D4)</f>
-        <v>42135</v>
+        <v>42138</v>
       </c>
       <c r="I4" s="84">
         <f>_xll.qlRateHelperLatestDate($D4)</f>
-        <v>42149</v>
+        <v>42152</v>
       </c>
       <c r="J4" s="72">
-        <v>2.199072302668147E-2</v>
+        <v>2.1990723026677705E-2</v>
       </c>
       <c r="K4" s="77"/>
     </row>
@@ -7948,7 +7946,7 @@
         <v>48</v>
       </c>
       <c r="D5" s="75" t="str">
-        <v>obj_00266</v>
+        <v>obj_002cd</v>
       </c>
       <c r="E5" s="75" t="str">
         <f>SUBSTITUTE(SUBSTITUTE(_xll.qlRateHelperQuoteName(D5),"LastFixing","D"),"Libor","")</f>
@@ -7964,20 +7962,20 @@
       </c>
       <c r="H5" s="83">
         <f>_xll.qlRateHelperEarliestDate($D5)</f>
-        <v>42135</v>
+        <v>42138</v>
       </c>
       <c r="I5" s="84">
         <f>_xll.qlRateHelperLatestDate($D5)</f>
-        <v>42156</v>
+        <v>42159</v>
       </c>
       <c r="J5" s="72">
-        <v>2.2485449200022385E-2</v>
+        <v>2.2485449200022371E-2</v>
       </c>
       <c r="K5" s="77"/>
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.2">
       <c r="D6" s="75" t="str">
-        <v>obj_00263</v>
+        <v>obj_002cc</v>
       </c>
       <c r="E6" s="75" t="str">
         <f>SUBSTITUTE(SUBSTITUTE(_xll.qlRateHelperQuoteName(D6),"LastFixing","D"),"Libor","")</f>
@@ -7993,28 +7991,28 @@
       </c>
       <c r="H6" s="83">
         <f>_xll.qlRateHelperEarliestDate($D6)</f>
-        <v>42135</v>
+        <v>42138</v>
       </c>
       <c r="I6" s="84">
         <f>_xll.qlRateHelperLatestDate($D6)</f>
-        <v>42166</v>
+        <v>42170</v>
       </c>
       <c r="J6" s="72">
-        <v>2.058200022462572E-2</v>
+        <v>2.0581420284760919E-2</v>
       </c>
       <c r="K6" s="77"/>
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.2">
       <c r="D7" s="75" t="str">
-        <v>obj_00265</v>
+        <v>obj_0026f</v>
       </c>
       <c r="E7" s="75" t="str">
         <f>SUBSTITUTE(SUBSTITUTE(_xll.qlRateHelperQuoteName(D7),"LastFixing","D"),"Libor","")</f>
-        <v>AUD2MD_Quote</v>
+        <v>AUDFUT3MM5_Quote</v>
       </c>
       <c r="F7" s="76">
         <f>_xll.qlRateHelperRate($D7)</f>
-        <v>2.12E-2</v>
+        <v>2.1649999999999947E-2</v>
       </c>
       <c r="G7" s="76">
         <f>IF(ISERROR(_xll.qlSwapRateHelperSpread($D7)),IF(ISERROR(_xll.qlFuturesRateHelperConvexityAdjustment($D7)),0,_xll.qlFuturesRateHelperConvexityAdjustment($D7)),_xll.qlSwapRateHelperSpread($D7))</f>
@@ -8022,28 +8020,28 @@
       </c>
       <c r="H7" s="83">
         <f>_xll.qlRateHelperEarliestDate($D7)</f>
-        <v>42135</v>
+        <v>42167</v>
       </c>
       <c r="I7" s="84">
         <f>_xll.qlRateHelperLatestDate($D7)</f>
-        <v>42198</v>
+        <v>42261</v>
       </c>
       <c r="J7" s="72">
-        <v>2.1161307073142656E-2</v>
+        <v>2.1474535434658069E-2</v>
       </c>
       <c r="K7" s="77"/>
     </row>
     <row r="8" spans="1:11" x14ac:dyDescent="0.2">
       <c r="D8" s="75" t="str">
-        <v>obj_00394</v>
+        <v>obj_00273</v>
       </c>
       <c r="E8" s="75" t="str">
         <f>SUBSTITUTE(SUBSTITUTE(_xll.qlRateHelperQuoteName(D8),"LastFixing","D"),"Libor","")</f>
-        <v>AUDFUT3MM5_Quote</v>
+        <v>AUDFUT3MU5_Quote</v>
       </c>
       <c r="F8" s="76">
         <f>_xll.qlRateHelperRate($D8)</f>
-        <v>2.1549999999999958E-2</v>
+        <v>2.1150000000000113E-2</v>
       </c>
       <c r="G8" s="76">
         <f>IF(ISERROR(_xll.qlSwapRateHelperSpread($D8)),IF(ISERROR(_xll.qlFuturesRateHelperConvexityAdjustment($D8)),0,_xll.qlFuturesRateHelperConvexityAdjustment($D8)),_xll.qlSwapRateHelperSpread($D8))</f>
@@ -8051,28 +8049,28 @@
       </c>
       <c r="H8" s="83">
         <f>_xll.qlRateHelperEarliestDate($D8)</f>
-        <v>42167</v>
+        <v>42258</v>
       </c>
       <c r="I8" s="84">
         <f>_xll.qlRateHelperLatestDate($D8)</f>
-        <v>42261</v>
+        <v>42349</v>
       </c>
       <c r="J8" s="72">
-        <v>2.126430830908628E-2</v>
+        <v>2.1293860020382357E-2</v>
       </c>
       <c r="K8" s="77"/>
     </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.2">
       <c r="D9" s="75" t="str">
-        <v>obj_00385</v>
+        <v>obj_00283</v>
       </c>
       <c r="E9" s="75" t="str">
         <f>SUBSTITUTE(SUBSTITUTE(_xll.qlRateHelperQuoteName(D9),"LastFixing","D"),"Libor","")</f>
-        <v>AUDFUT3MU5_Quote</v>
+        <v>AUDFUT3MZ5_Quote</v>
       </c>
       <c r="F9" s="76">
         <f>_xll.qlRateHelperRate($D9)</f>
-        <v>2.1049999999999902E-2</v>
+        <v>2.1150000000000113E-2</v>
       </c>
       <c r="G9" s="76">
         <f>IF(ISERROR(_xll.qlSwapRateHelperSpread($D9)),IF(ISERROR(_xll.qlFuturesRateHelperConvexityAdjustment($D9)),0,_xll.qlFuturesRateHelperConvexityAdjustment($D9)),_xll.qlSwapRateHelperSpread($D9))</f>
@@ -8080,28 +8078,28 @@
       </c>
       <c r="H9" s="83">
         <f>_xll.qlRateHelperEarliestDate($D9)</f>
-        <v>42258</v>
+        <v>42349</v>
       </c>
       <c r="I9" s="84">
         <f>_xll.qlRateHelperLatestDate($D9)</f>
-        <v>42349</v>
+        <v>42440</v>
       </c>
       <c r="J9" s="72">
-        <v>2.1146951703140075E-2</v>
+        <v>2.1233767812008888E-2</v>
       </c>
       <c r="K9" s="77"/>
     </row>
     <row r="10" spans="1:11" x14ac:dyDescent="0.2">
       <c r="D10" s="75" t="str">
-        <v>obj_00397</v>
+        <v>obj_0027d</v>
       </c>
       <c r="E10" s="75" t="str">
         <f>SUBSTITUTE(SUBSTITUTE(_xll.qlRateHelperQuoteName(D10),"LastFixing","D"),"Libor","")</f>
-        <v>AUDFUT3MZ5_Quote</v>
+        <v>AUDFUT3MH6_Quote</v>
       </c>
       <c r="F10" s="76">
         <f>_xll.qlRateHelperRate($D10)</f>
-        <v>2.1150000000000113E-2</v>
+        <v>2.1649999999999947E-2</v>
       </c>
       <c r="G10" s="76">
         <f>IF(ISERROR(_xll.qlSwapRateHelperSpread($D10)),IF(ISERROR(_xll.qlFuturesRateHelperConvexityAdjustment($D10)),0,_xll.qlFuturesRateHelperConvexityAdjustment($D10)),_xll.qlSwapRateHelperSpread($D10))</f>
@@ -8109,28 +8107,28 @@
       </c>
       <c r="H10" s="83">
         <f>_xll.qlRateHelperEarliestDate($D10)</f>
-        <v>42349</v>
+        <v>42440</v>
       </c>
       <c r="I10" s="84">
         <f>_xll.qlRateHelperLatestDate($D10)</f>
-        <v>42440</v>
+        <v>42535</v>
       </c>
       <c r="J10" s="72">
-        <v>2.1131282227541705E-2</v>
+        <v>2.1318828044998739E-2</v>
       </c>
       <c r="K10" s="77"/>
     </row>
     <row r="11" spans="1:11" x14ac:dyDescent="0.2">
       <c r="D11" s="75" t="str">
-        <v>obj_0039f</v>
+        <v>obj_00263</v>
       </c>
       <c r="E11" s="75" t="str">
         <f>SUBSTITUTE(SUBSTITUTE(_xll.qlRateHelperQuoteName(D11),"LastFixing","D"),"Libor","")</f>
-        <v>AUDFUT3MH6_Quote</v>
+        <v>AUDFUT3MM6_Quote</v>
       </c>
       <c r="F11" s="76">
         <f>_xll.qlRateHelperRate($D11)</f>
-        <v>2.1549999999999958E-2</v>
+        <v>2.2249999999999992E-2</v>
       </c>
       <c r="G11" s="76">
         <f>IF(ISERROR(_xll.qlSwapRateHelperSpread($D11)),IF(ISERROR(_xll.qlFuturesRateHelperConvexityAdjustment($D11)),0,_xll.qlFuturesRateHelperConvexityAdjustment($D11)),_xll.qlSwapRateHelperSpread($D11))</f>
@@ -8138,28 +8136,28 @@
       </c>
       <c r="H11" s="83">
         <f>_xll.qlRateHelperEarliestDate($D11)</f>
-        <v>42440</v>
+        <v>42531</v>
       </c>
       <c r="I11" s="84">
         <f>_xll.qlRateHelperLatestDate($D11)</f>
-        <v>42535</v>
+        <v>42625</v>
       </c>
       <c r="J11" s="72">
-        <v>2.1216427609261884E-2</v>
+        <v>2.148341355455172E-2</v>
       </c>
       <c r="K11" s="77"/>
     </row>
     <row r="12" spans="1:11" x14ac:dyDescent="0.2">
       <c r="D12" s="75" t="str">
-        <v>obj_00392</v>
+        <v>obj_0027c</v>
       </c>
       <c r="E12" s="75" t="str">
         <f>SUBSTITUTE(SUBSTITUTE(_xll.qlRateHelperQuoteName(D12),"LastFixing","D"),"Libor","")</f>
-        <v>AUDFUT3MM6_Quote</v>
+        <v>AUDFUT3MU6_Quote</v>
       </c>
       <c r="F12" s="76">
         <f>_xll.qlRateHelperRate($D12)</f>
-        <v>2.2150000000000003E-2</v>
+        <v>2.3050000000000015E-2</v>
       </c>
       <c r="G12" s="76">
         <f>IF(ISERROR(_xll.qlSwapRateHelperSpread($D12)),IF(ISERROR(_xll.qlFuturesRateHelperConvexityAdjustment($D12)),0,_xll.qlFuturesRateHelperConvexityAdjustment($D12)),_xll.qlSwapRateHelperSpread($D12))</f>
@@ -8167,28 +8165,28 @@
       </c>
       <c r="H12" s="83">
         <f>_xll.qlRateHelperEarliestDate($D12)</f>
-        <v>42531</v>
+        <v>42622</v>
       </c>
       <c r="I12" s="84">
         <f>_xll.qlRateHelperLatestDate($D12)</f>
-        <v>42625</v>
+        <v>42713</v>
       </c>
       <c r="J12" s="72">
-        <v>2.1380550173858173E-2</v>
+        <v>2.1716283183511837E-2</v>
       </c>
       <c r="K12" s="77"/>
     </row>
     <row r="13" spans="1:11" x14ac:dyDescent="0.2">
       <c r="D13" s="75" t="str">
-        <v>obj_0038f</v>
+        <v>obj_002bf</v>
       </c>
       <c r="E13" s="75" t="str">
         <f>SUBSTITUTE(SUBSTITUTE(_xll.qlRateHelperQuoteName(D13),"LastFixing","D"),"Libor","")</f>
-        <v>AUDFUT3MU6_Quote</v>
+        <v>AUDQM3AB2Y_Quote</v>
       </c>
       <c r="F13" s="76">
         <f>_xll.qlRateHelperRate($D13)</f>
-        <v>2.2849999999999926E-2</v>
+        <v>2.2599999999999999E-2</v>
       </c>
       <c r="G13" s="76">
         <f>IF(ISERROR(_xll.qlSwapRateHelperSpread($D13)),IF(ISERROR(_xll.qlFuturesRateHelperConvexityAdjustment($D13)),0,_xll.qlFuturesRateHelperConvexityAdjustment($D13)),_xll.qlSwapRateHelperSpread($D13))</f>
@@ -8196,28 +8194,28 @@
       </c>
       <c r="H13" s="83">
         <f>_xll.qlRateHelperEarliestDate($D13)</f>
-        <v>42622</v>
+        <v>42139</v>
       </c>
       <c r="I13" s="84">
         <f>_xll.qlRateHelperLatestDate($D13)</f>
-        <v>42713</v>
+        <v>42870</v>
       </c>
       <c r="J13" s="72">
-        <v>2.1597081670140534E-2</v>
+        <v>2.2551926044568637E-2</v>
       </c>
       <c r="K13" s="77"/>
     </row>
     <row r="14" spans="1:11" x14ac:dyDescent="0.2">
       <c r="D14" s="75" t="str">
-        <v>obj_003aa</v>
+        <v>obj_002ba</v>
       </c>
       <c r="E14" s="75" t="str">
         <f>SUBSTITUTE(SUBSTITUTE(_xll.qlRateHelperQuoteName(D14),"LastFixing","D"),"Libor","")</f>
-        <v>AUDQM3AB2Y_Quote</v>
+        <v>AUDQM3AB3Y_Quote</v>
       </c>
       <c r="F14" s="76">
         <f>_xll.qlRateHelperRate($D14)</f>
-        <v>2.205E-2</v>
+        <v>2.4125000000000004E-2</v>
       </c>
       <c r="G14" s="76">
         <f>IF(ISERROR(_xll.qlSwapRateHelperSpread($D14)),IF(ISERROR(_xll.qlFuturesRateHelperConvexityAdjustment($D14)),0,_xll.qlFuturesRateHelperConvexityAdjustment($D14)),_xll.qlSwapRateHelperSpread($D14))</f>
@@ -8225,28 +8223,28 @@
       </c>
       <c r="H14" s="83">
         <f>_xll.qlRateHelperEarliestDate($D14)</f>
-        <v>42136</v>
+        <v>42139</v>
       </c>
       <c r="I14" s="84">
         <f>_xll.qlRateHelperLatestDate($D14)</f>
-        <v>42867</v>
+        <v>43235</v>
       </c>
       <c r="J14" s="72">
-        <v>2.2000154074826372E-2</v>
+        <v>2.4101635885697248E-2</v>
       </c>
       <c r="K14" s="77"/>
     </row>
     <row r="15" spans="1:11" x14ac:dyDescent="0.2">
       <c r="D15" s="75" t="str">
-        <v>obj_003a9</v>
+        <v>obj_002aa</v>
       </c>
       <c r="E15" s="75" t="str">
         <f>SUBSTITUTE(SUBSTITUTE(_xll.qlRateHelperQuoteName(D15),"LastFixing","D"),"Libor","")</f>
-        <v>AUDQM3AB3Y_Quote</v>
+        <v>AUDSM6AB4Y_Quote</v>
       </c>
       <c r="F15" s="76">
         <f>_xll.qlRateHelperRate($D15)</f>
-        <v>2.3300000000000001E-2</v>
+        <v>2.6699999999999998E-2</v>
       </c>
       <c r="G15" s="76">
         <f>IF(ISERROR(_xll.qlSwapRateHelperSpread($D15)),IF(ISERROR(_xll.qlFuturesRateHelperConvexityAdjustment($D15)),0,_xll.qlFuturesRateHelperConvexityAdjustment($D15)),_xll.qlSwapRateHelperSpread($D15))</f>
@@ -8254,28 +8252,28 @@
       </c>
       <c r="H15" s="83">
         <f>_xll.qlRateHelperEarliestDate($D15)</f>
-        <v>42136</v>
+        <v>42139</v>
       </c>
       <c r="I15" s="84">
         <f>_xll.qlRateHelperLatestDate($D15)</f>
-        <v>43234</v>
+        <v>43600</v>
       </c>
       <c r="J15" s="72">
-        <v>2.3269739582871315E-2</v>
+        <v>2.666584785797365E-2</v>
       </c>
       <c r="K15" s="77"/>
     </row>
     <row r="16" spans="1:11" x14ac:dyDescent="0.2">
       <c r="D16" s="75" t="str">
-        <v>obj_003ab</v>
+        <v>obj_002a6</v>
       </c>
       <c r="E16" s="75" t="str">
         <f>SUBSTITUTE(SUBSTITUTE(_xll.qlRateHelperQuoteName(D16),"LastFixing","D"),"Libor","")</f>
-        <v>AUDSM6AB4Y_Quote</v>
+        <v>AUDSM6AB5Y_Quote</v>
       </c>
       <c r="F16" s="76">
         <f>_xll.qlRateHelperRate($D16)</f>
-        <v>2.5675E-2</v>
+        <v>2.8174999999999999E-2</v>
       </c>
       <c r="G16" s="76">
         <f>IF(ISERROR(_xll.qlSwapRateHelperSpread($D16)),IF(ISERROR(_xll.qlFuturesRateHelperConvexityAdjustment($D16)),0,_xll.qlFuturesRateHelperConvexityAdjustment($D16)),_xll.qlSwapRateHelperSpread($D16))</f>
@@ -8283,27 +8281,27 @@
       </c>
       <c r="H16" s="83">
         <f>_xll.qlRateHelperEarliestDate($D16)</f>
-        <v>42136</v>
+        <v>42139</v>
       </c>
       <c r="I16" s="84">
         <f>_xll.qlRateHelperLatestDate($D16)</f>
-        <v>43598</v>
+        <v>43966</v>
       </c>
       <c r="J16" s="72">
-        <v>2.5632785108581555E-2</v>
+        <v>2.8184965050177289E-2</v>
       </c>
     </row>
     <row r="17" spans="4:10" x14ac:dyDescent="0.2">
       <c r="D17" s="75" t="str">
-        <v>obj_003ac</v>
+        <v>obj_002b0</v>
       </c>
       <c r="E17" s="75" t="str">
         <f>SUBSTITUTE(SUBSTITUTE(_xll.qlRateHelperQuoteName(D17),"LastFixing","D"),"Libor","")</f>
-        <v>AUDSM6AB5Y_Quote</v>
+        <v>AUDSM6AB7Y_Quote</v>
       </c>
       <c r="F17" s="76">
         <f>_xll.qlRateHelperRate($D17)</f>
-        <v>2.6974999999999999E-2</v>
+        <v>3.0724999999999999E-2</v>
       </c>
       <c r="G17" s="76">
         <f>IF(ISERROR(_xll.qlSwapRateHelperSpread($D17)),IF(ISERROR(_xll.qlFuturesRateHelperConvexityAdjustment($D17)),0,_xll.qlFuturesRateHelperConvexityAdjustment($D17)),_xll.qlSwapRateHelperSpread($D17))</f>
@@ -8311,27 +8309,27 @@
       </c>
       <c r="H17" s="83">
         <f>_xll.qlRateHelperEarliestDate($D17)</f>
-        <v>42136</v>
+        <v>42139</v>
       </c>
       <c r="I17" s="84">
         <f>_xll.qlRateHelperLatestDate($D17)</f>
-        <v>43963</v>
+        <v>44697</v>
       </c>
       <c r="J17" s="72">
-        <v>2.6969326886725882E-2</v>
+        <v>3.0866430267649264E-2</v>
       </c>
     </row>
     <row r="18" spans="4:10" x14ac:dyDescent="0.2">
       <c r="D18" s="75" t="str">
-        <v>obj_003b9</v>
+        <v>obj_002b3</v>
       </c>
       <c r="E18" s="75" t="str">
         <f>SUBSTITUTE(SUBSTITUTE(_xll.qlRateHelperQuoteName(D18),"LastFixing","D"),"Libor","")</f>
-        <v>AUDSM6AB7Y_Quote</v>
+        <v>AUDSM6AB10Y_Quote</v>
       </c>
       <c r="F18" s="76">
         <f>_xll.qlRateHelperRate($D18)</f>
-        <v>2.92E-2</v>
+        <v>3.3399999999999999E-2</v>
       </c>
       <c r="G18" s="76">
         <f>IF(ISERROR(_xll.qlSwapRateHelperSpread($D18)),IF(ISERROR(_xll.qlFuturesRateHelperConvexityAdjustment($D18)),0,_xll.qlFuturesRateHelperConvexityAdjustment($D18)),_xll.qlSwapRateHelperSpread($D18))</f>
@@ -8339,27 +8337,27 @@
       </c>
       <c r="H18" s="83">
         <f>_xll.qlRateHelperEarliestDate($D18)</f>
-        <v>42136</v>
+        <v>42139</v>
       </c>
       <c r="I18" s="84">
         <f>_xll.qlRateHelperLatestDate($D18)</f>
-        <v>44693</v>
+        <v>45792</v>
       </c>
       <c r="J18" s="72">
-        <v>2.9300732956604889E-2</v>
+        <v>3.3769600259993066E-2</v>
       </c>
     </row>
     <row r="19" spans="4:10" x14ac:dyDescent="0.2">
       <c r="D19" s="75" t="str">
-        <v>obj_003c0</v>
+        <v>obj_0029b</v>
       </c>
       <c r="E19" s="75" t="str">
         <f>SUBSTITUTE(SUBSTITUTE(_xll.qlRateHelperQuoteName(D19),"LastFixing","D"),"Libor","")</f>
-        <v>AUDSM6AB10Y_Quote</v>
+        <v>AUDSM6AB12Y_Quote</v>
       </c>
       <c r="F19" s="76">
         <f>_xll.qlRateHelperRate($D19)</f>
-        <v>3.1574999999999999E-2</v>
+        <v>3.4750000000000003E-2</v>
       </c>
       <c r="G19" s="76">
         <f>IF(ISERROR(_xll.qlSwapRateHelperSpread($D19)),IF(ISERROR(_xll.qlFuturesRateHelperConvexityAdjustment($D19)),0,_xll.qlFuturesRateHelperConvexityAdjustment($D19)),_xll.qlSwapRateHelperSpread($D19))</f>
@@ -8367,27 +8365,27 @@
       </c>
       <c r="H19" s="83">
         <f>_xll.qlRateHelperEarliestDate($D19)</f>
-        <v>42136</v>
+        <v>42139</v>
       </c>
       <c r="I19" s="84">
         <f>_xll.qlRateHelperLatestDate($D19)</f>
-        <v>45789</v>
+        <v>46524</v>
       </c>
       <c r="J19" s="72">
-        <v>3.1863898345015705E-2</v>
+        <v>3.5285559372487986E-2</v>
       </c>
     </row>
     <row r="20" spans="4:10" x14ac:dyDescent="0.2">
       <c r="D20" s="75" t="str">
-        <v>obj_003c6</v>
+        <v>obj_002b5</v>
       </c>
       <c r="E20" s="75" t="str">
         <f>SUBSTITUTE(SUBSTITUTE(_xll.qlRateHelperQuoteName(D20),"LastFixing","D"),"Libor","")</f>
-        <v>AUDSM6AB12Y_Quote</v>
+        <v>AUDSM6AB15Y_Quote</v>
       </c>
       <c r="F20" s="76">
         <f>_xll.qlRateHelperRate($D20)</f>
-        <v>3.2850000000000004E-2</v>
+        <v>3.61E-2</v>
       </c>
       <c r="G20" s="76">
         <f>IF(ISERROR(_xll.qlSwapRateHelperSpread($D20)),IF(ISERROR(_xll.qlFuturesRateHelperConvexityAdjustment($D20)),0,_xll.qlFuturesRateHelperConvexityAdjustment($D20)),_xll.qlSwapRateHelperSpread($D20))</f>
@@ -8395,27 +8393,27 @@
       </c>
       <c r="H20" s="83">
         <f>_xll.qlRateHelperEarliestDate($D20)</f>
-        <v>42136</v>
+        <v>42139</v>
       </c>
       <c r="I20" s="84">
         <f>_xll.qlRateHelperLatestDate($D20)</f>
-        <v>46519</v>
+        <v>47618</v>
       </c>
       <c r="J20" s="72">
-        <v>3.3290099555338418E-2</v>
+        <v>3.6832582119064219E-2</v>
       </c>
     </row>
     <row r="21" spans="4:10" x14ac:dyDescent="0.2">
       <c r="D21" s="75" t="str">
-        <v>obj_003b0</v>
+        <v>obj_002b6</v>
       </c>
       <c r="E21" s="75" t="str">
         <f>SUBSTITUTE(SUBSTITUTE(_xll.qlRateHelperQuoteName(D21),"LastFixing","D"),"Libor","")</f>
-        <v>AUDSM6AB15Y_Quote</v>
+        <v>AUDSM6AB20Y_Quote</v>
       </c>
       <c r="F21" s="76">
         <f>_xll.qlRateHelperRate($D21)</f>
-        <v>3.4200000000000001E-2</v>
+        <v>3.7025000000000002E-2</v>
       </c>
       <c r="G21" s="76">
         <f>IF(ISERROR(_xll.qlSwapRateHelperSpread($D21)),IF(ISERROR(_xll.qlFuturesRateHelperConvexityAdjustment($D21)),0,_xll.qlFuturesRateHelperConvexityAdjustment($D21)),_xll.qlSwapRateHelperSpread($D21))</f>
@@ -8423,27 +8421,27 @@
       </c>
       <c r="H21" s="83">
         <f>_xll.qlRateHelperEarliestDate($D21)</f>
-        <v>42136</v>
+        <v>42139</v>
       </c>
       <c r="I21" s="84">
         <f>_xll.qlRateHelperLatestDate($D21)</f>
-        <v>47616</v>
+        <v>49444</v>
       </c>
       <c r="J21" s="72">
-        <v>3.4837018000288406E-2</v>
+        <v>3.7839152057244745E-2</v>
       </c>
     </row>
     <row r="22" spans="4:10" x14ac:dyDescent="0.2">
       <c r="D22" s="75" t="str">
-        <v>obj_003c7</v>
+        <v>obj_0029c</v>
       </c>
       <c r="E22" s="75" t="str">
         <f>SUBSTITUTE(SUBSTITUTE(_xll.qlRateHelperQuoteName(D22),"LastFixing","D"),"Libor","")</f>
-        <v>AUDSM6AB20Y_Quote</v>
+        <v>AUDSM6AB30Y_Quote</v>
       </c>
       <c r="F22" s="76">
         <f>_xll.qlRateHelperRate($D22)</f>
-        <v>3.5125000000000003E-2</v>
+        <v>3.7499999999999999E-2</v>
       </c>
       <c r="G22" s="76">
         <f>IF(ISERROR(_xll.qlSwapRateHelperSpread($D22)),IF(ISERROR(_xll.qlFuturesRateHelperConvexityAdjustment($D22)),0,_xll.qlFuturesRateHelperConvexityAdjustment($D22)),_xll.qlSwapRateHelperSpread($D22))</f>
@@ -8451,42 +8449,42 @@
       </c>
       <c r="H22" s="83">
         <f>_xll.qlRateHelperEarliestDate($D22)</f>
-        <v>42136</v>
+        <v>42139</v>
       </c>
       <c r="I22" s="84">
         <f>_xll.qlRateHelperLatestDate($D22)</f>
-        <v>49443</v>
+        <v>53097</v>
       </c>
       <c r="J22" s="72">
-        <v>3.5852769597767065E-2</v>
+        <v>3.8196471968635168E-2</v>
       </c>
     </row>
     <row r="23" spans="4:10" x14ac:dyDescent="0.2">
-      <c r="D23" s="75" t="str">
-        <v>obj_003b6</v>
-      </c>
-      <c r="E23" s="75" t="str">
+      <c r="D23" s="75" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="E23" s="75" t="e">
         <f>SUBSTITUTE(SUBSTITUTE(_xll.qlRateHelperQuoteName(D23),"LastFixing","D"),"Libor","")</f>
-        <v>AUDSM6AB30Y_Quote</v>
-      </c>
-      <c r="F23" s="76">
+        <v>#VALUE!</v>
+      </c>
+      <c r="F23" s="76" t="e">
         <f>_xll.qlRateHelperRate($D23)</f>
-        <v>3.56E-2</v>
+        <v>#VALUE!</v>
       </c>
       <c r="G23" s="76">
         <f>IF(ISERROR(_xll.qlSwapRateHelperSpread($D23)),IF(ISERROR(_xll.qlFuturesRateHelperConvexityAdjustment($D23)),0,_xll.qlFuturesRateHelperConvexityAdjustment($D23)),_xll.qlSwapRateHelperSpread($D23))</f>
         <v>0</v>
       </c>
-      <c r="H23" s="83">
+      <c r="H23" s="83" t="e">
         <f>_xll.qlRateHelperEarliestDate($D23)</f>
-        <v>42136</v>
-      </c>
-      <c r="I23" s="84">
+        <v>#VALUE!</v>
+      </c>
+      <c r="I23" s="84" t="e">
         <f>_xll.qlRateHelperLatestDate($D23)</f>
-        <v>53094</v>
-      </c>
-      <c r="J23" s="72">
-        <v>3.6232381509052253E-2</v>
+        <v>#VALUE!</v>
+      </c>
+      <c r="J23" s="72" t="e">
+        <v>#N/A</v>
       </c>
     </row>
     <row r="24" spans="4:10" x14ac:dyDescent="0.2">
@@ -11499,7 +11497,7 @@
       </c>
       <c r="J3" s="49" t="str">
         <f>_xll.qlDepositRateHelper(,I3,H3,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>obj_00267#0002</v>
+        <v>obj_002c0#0001</v>
       </c>
       <c r="K3" s="53" t="str">
         <f>_xll.ohRangeRetrieveError(J3)</f>
@@ -11529,7 +11527,7 @@
       </c>
       <c r="H4" s="50" t="str">
         <f>_xll.qlIborIndex(,,"1D",C4,Currency,D4,E4,F4,G4,,,Trigger,ObjectOverwrite)</f>
-        <v>obj_0024b#0002</v>
+        <v>obj_00286#0001</v>
       </c>
       <c r="I4" s="50" t="str">
         <f t="shared" si="0"/>
@@ -11537,7 +11535,7 @@
       </c>
       <c r="J4" s="49" t="str">
         <f>_xll.qlDepositRateHelper(,I4,H4,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>obj_0024e#0002</v>
+        <v>obj_00288#0001</v>
       </c>
       <c r="K4" s="53"/>
       <c r="L4" s="47"/>
@@ -11564,7 +11562,7 @@
       </c>
       <c r="H5" s="50" t="str">
         <f>_xll.qlIborIndex(,,"1D",C5,Currency,D5,E5,F5,G5,,,Trigger,ObjectOverwrite)</f>
-        <v>obj_0024c#0003</v>
+        <v>obj_0025b#0001</v>
       </c>
       <c r="I5" s="50" t="str">
         <f t="shared" si="0"/>
@@ -11572,7 +11570,7 @@
       </c>
       <c r="J5" s="49" t="str">
         <f>_xll.qlDepositRateHelper(,I5,H5,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>obj_0024d#0003</v>
+        <v>obj_00287#0001</v>
       </c>
       <c r="K5" s="53"/>
       <c r="L5" s="47"/>
@@ -11599,7 +11597,7 @@
       </c>
       <c r="H6" s="50" t="str">
         <f>_xll.qlIborIndex(,,"1W",C6,Currency,D6,E6,F6,G6,,,Trigger,ObjectOverwrite)</f>
-        <v>obj_00252#0002</v>
+        <v>obj_0028e#0001</v>
       </c>
       <c r="I6" s="50" t="str">
         <f t="shared" si="0"/>
@@ -11607,7 +11605,7 @@
       </c>
       <c r="J6" s="49" t="str">
         <f>_xll.qlDepositRateHelper(,I6,H6,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>obj_00255#0002</v>
+        <v>obj_00294#0001</v>
       </c>
       <c r="K6" s="48" t="str">
         <f>_xll.ohRangeRetrieveError(J6)</f>
@@ -11637,7 +11635,7 @@
       </c>
       <c r="H7" s="50" t="str">
         <f>_xll.qlIborIndex(,,B7,C7,Currency,D7,E7,F7,G7,,,Trigger,ObjectOverwrite)</f>
-        <v>obj_00256#0002</v>
+        <v>obj_00296#0001</v>
       </c>
       <c r="I7" s="50" t="str">
         <f t="shared" si="0"/>
@@ -11645,7 +11643,7 @@
       </c>
       <c r="J7" s="49" t="str">
         <f>_xll.qlDepositRateHelper(,I7,H7,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>obj_00262#0002</v>
+        <v>obj_002c8#0001</v>
       </c>
       <c r="K7" s="48" t="str">
         <f>_xll.ohRangeRetrieveError(J7)</f>
@@ -11675,7 +11673,7 @@
       </c>
       <c r="H8" s="50" t="str">
         <f>_xll.qlIborIndex(,,B8,C8,Currency,D8,E8,F8,G8,,,Trigger,ObjectOverwrite)</f>
-        <v>obj_00258#0002</v>
+        <v>obj_0028c#0001</v>
       </c>
       <c r="I8" s="50" t="str">
         <f t="shared" si="0"/>
@@ -11683,7 +11681,7 @@
       </c>
       <c r="J8" s="49" t="str">
         <f>_xll.qlDepositRateHelper(,I8,H8,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>obj_00266#0002</v>
+        <v>obj_002cd#0001</v>
       </c>
       <c r="K8" s="48" t="str">
         <f>_xll.ohRangeRetrieveError(J8)</f>
@@ -11713,7 +11711,7 @@
       </c>
       <c r="H9" s="50" t="str">
         <f>_xll.qlIborIndex(,,B9,C9,Currency,D9,E9,F9,G9,,,Trigger,ObjectOverwrite)</f>
-        <v>obj_00259#0002</v>
+        <v>obj_0028f#0001</v>
       </c>
       <c r="I9" s="50" t="str">
         <f t="shared" si="0"/>
@@ -11721,7 +11719,7 @@
       </c>
       <c r="J9" s="49" t="str">
         <f>_xll.qlDepositRateHelper(,I9,H9,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>obj_00263#0002</v>
+        <v>obj_002cc#0001</v>
       </c>
       <c r="K9" s="48" t="str">
         <f>_xll.ohRangeRetrieveError(J9)</f>
@@ -11751,7 +11749,7 @@
       </c>
       <c r="H10" s="50" t="str">
         <f>_xll.qlIborIndex(,,B10,C10,Currency,D10,E10,F10,G10,,,Trigger,ObjectOverwrite)</f>
-        <v>obj_0025d#0002</v>
+        <v>obj_00297#0001</v>
       </c>
       <c r="I10" s="50" t="str">
         <f t="shared" si="0"/>
@@ -11759,7 +11757,7 @@
       </c>
       <c r="J10" s="49" t="str">
         <f>_xll.qlDepositRateHelper(,I10,H10,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>obj_00265#0002</v>
+        <v>obj_002c9#0001</v>
       </c>
       <c r="K10" s="48" t="str">
         <f>_xll.ohRangeRetrieveError(J10)</f>
@@ -11789,7 +11787,7 @@
       </c>
       <c r="H11" s="50" t="str">
         <f>_xll.qlIborIndex(,,B11,C11,Currency,D11,E11,F11,G11,,,Trigger,ObjectOverwrite)</f>
-        <v>obj_00250#0002</v>
+        <v>obj_00289#0001</v>
       </c>
       <c r="I11" s="50" t="str">
         <f t="shared" si="0"/>
@@ -11797,7 +11795,7 @@
       </c>
       <c r="J11" s="49" t="str">
         <f>_xll.qlDepositRateHelper(,I11,H11,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>obj_0026e#0002</v>
+        <v>obj_002c7#0001</v>
       </c>
       <c r="K11" s="48" t="str">
         <f>_xll.ohRangeRetrieveError(J11)</f>
@@ -11827,7 +11825,7 @@
       </c>
       <c r="H12" s="50" t="str">
         <f>_xll.qlIborIndex(,,B12,C12,Currency,D12,E12,F12,G12,,,Trigger,ObjectOverwrite)</f>
-        <v>obj_00253#0002</v>
+        <v>obj_00290#0001</v>
       </c>
       <c r="I12" s="50" t="str">
         <f t="shared" si="0"/>
@@ -11835,7 +11833,7 @@
       </c>
       <c r="J12" s="49" t="str">
         <f>_xll.qlDepositRateHelper(,I12,H12,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>obj_0026b#0002</v>
+        <v>obj_002c1#0001</v>
       </c>
       <c r="K12" s="48" t="str">
         <f>_xll.ohRangeRetrieveError(J12)</f>
@@ -11865,7 +11863,7 @@
       </c>
       <c r="H13" s="50" t="str">
         <f>_xll.qlIborIndex(,,B13,C13,Currency,D13,E13,F13,G13,,,Trigger,ObjectOverwrite)</f>
-        <v>obj_0025a#0002</v>
+        <v>obj_00291#0001</v>
       </c>
       <c r="I13" s="50" t="str">
         <f t="shared" si="0"/>
@@ -11873,7 +11871,7 @@
       </c>
       <c r="J13" s="49" t="str">
         <f>_xll.qlDepositRateHelper(,I13,H13,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>obj_0026f#0002</v>
+        <v>obj_002cb#0001</v>
       </c>
       <c r="K13" s="48" t="str">
         <f>_xll.ohRangeRetrieveError(J13)</f>
@@ -11903,7 +11901,7 @@
       </c>
       <c r="H14" s="50" t="str">
         <f>_xll.qlIborIndex(,,B14,C14,Currency,D14,E14,F14,G14,,,Trigger,ObjectOverwrite)</f>
-        <v>obj_00260#0002</v>
+        <v>obj_0028d#0001</v>
       </c>
       <c r="I14" s="50" t="str">
         <f t="shared" si="0"/>
@@ -11911,7 +11909,7 @@
       </c>
       <c r="J14" s="49" t="str">
         <f>_xll.qlDepositRateHelper(,I14,H14,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>obj_0026d#0002</v>
+        <v>obj_002c3#0001</v>
       </c>
       <c r="K14" s="48" t="str">
         <f>_xll.ohRangeRetrieveError(J14)</f>
@@ -11941,7 +11939,7 @@
       </c>
       <c r="H15" s="50" t="str">
         <f>_xll.qlIborIndex(,,B15,C15,Currency,D15,E15,F15,G15,,,Trigger,ObjectOverwrite)</f>
-        <v>obj_0025b#0002</v>
+        <v>obj_00293#0001</v>
       </c>
       <c r="I15" s="50" t="str">
         <f t="shared" si="0"/>
@@ -11949,7 +11947,7 @@
       </c>
       <c r="J15" s="49" t="str">
         <f>_xll.qlDepositRateHelper(,I15,H15,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>obj_00264#0002</v>
+        <v>obj_002c5#0001</v>
       </c>
       <c r="K15" s="53" t="str">
         <f>_xll.ohRangeRetrieveError(J15)</f>
@@ -11979,7 +11977,7 @@
       </c>
       <c r="H16" s="50" t="str">
         <f>_xll.qlIborIndex(,,B16,C16,Currency,D16,E16,F16,G16,,,Trigger,ObjectOverwrite)</f>
-        <v>obj_0025f#0002</v>
+        <v>obj_0028a#0001</v>
       </c>
       <c r="I16" s="50" t="str">
         <f t="shared" si="0"/>
@@ -11987,7 +11985,7 @@
       </c>
       <c r="J16" s="49" t="str">
         <f>_xll.qlDepositRateHelper(,I16,H16,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>obj_00261#0002</v>
+        <v>obj_002c4#0001</v>
       </c>
       <c r="K16" s="48" t="str">
         <f>_xll.ohRangeRetrieveError(J16)</f>
@@ -12017,7 +12015,7 @@
       </c>
       <c r="H17" s="50" t="str">
         <f>_xll.qlIborIndex(,,B17,C17,Currency,D17,E17,F17,G17,,,Trigger,ObjectOverwrite)</f>
-        <v>obj_00254#0002</v>
+        <v>obj_00292#0001</v>
       </c>
       <c r="I17" s="50" t="str">
         <f t="shared" si="0"/>
@@ -12025,7 +12023,7 @@
       </c>
       <c r="J17" s="49" t="str">
         <f>_xll.qlDepositRateHelper(,I17,H17,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>obj_00269#0002</v>
+        <v>obj_002ca#0001</v>
       </c>
       <c r="K17" s="48" t="str">
         <f>_xll.ohRangeRetrieveError(J17)</f>
@@ -12055,7 +12053,7 @@
       </c>
       <c r="H18" s="50" t="str">
         <f>_xll.qlIborIndex(,,B18,C18,Currency,D18,E18,F18,G18,,,Trigger,ObjectOverwrite)</f>
-        <v>obj_0025c#0002</v>
+        <v>obj_00295#0001</v>
       </c>
       <c r="I18" s="50" t="str">
         <f t="shared" si="0"/>
@@ -12063,7 +12061,7 @@
       </c>
       <c r="J18" s="49" t="str">
         <f>_xll.qlDepositRateHelper(,I18,H18,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>obj_0026c#0002</v>
+        <v>obj_002c2#0001</v>
       </c>
       <c r="K18" s="48" t="str">
         <f>_xll.ohRangeRetrieveError(J18)</f>
@@ -12093,7 +12091,7 @@
       </c>
       <c r="H19" s="50" t="str">
         <f>_xll.qlIborIndex(,,B19,C19,Currency,D19,E19,F19,G19,,,Trigger,ObjectOverwrite)</f>
-        <v>obj_00257#0002</v>
+        <v>obj_00299#0001</v>
       </c>
       <c r="I19" s="50" t="str">
         <f t="shared" si="0"/>
@@ -12101,7 +12099,7 @@
       </c>
       <c r="J19" s="49" t="str">
         <f>_xll.qlDepositRateHelper(,I19,H19,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>obj_00268#0002</v>
+        <v>obj_002c6#0001</v>
       </c>
       <c r="K19" s="48" t="str">
         <f>_xll.ohRangeRetrieveError(J19)</f>
@@ -12131,7 +12129,7 @@
       </c>
       <c r="H20" s="50" t="str">
         <f>_xll.qlIborIndex(,,B20,C20,Currency,D20,E20,F20,G20,,,Trigger,ObjectOverwrite)</f>
-        <v>obj_00251#0002</v>
+        <v>obj_0028b#0001</v>
       </c>
       <c r="I20" s="50" t="str">
         <f t="shared" si="0"/>
@@ -12139,7 +12137,7 @@
       </c>
       <c r="J20" s="49" t="str">
         <f>_xll.qlDepositRateHelper(,I20,H20,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>obj_0026a#0002</v>
+        <v>obj_002ce#0001</v>
       </c>
       <c r="K20" s="48"/>
       <c r="L20" s="47"/>
@@ -12268,7 +12266,7 @@
       <c r="H3" s="63"/>
       <c r="I3" s="133" t="str">
         <f>_xll.qlIborIndex(,FamilyName,IndexTenor,1,Currency,Calendar,"Half-Month Modified Following",TRUE,"actual/365 (fixed)",,,Trigger,ObjectOverwrite)</f>
-        <v>obj_0037a#0001</v>
+        <v>obj_0025a#0001</v>
       </c>
       <c r="J3" s="63"/>
       <c r="K3" s="47"/>
@@ -12319,7 +12317,7 @@
       </c>
       <c r="I5" s="134" t="str">
         <f>_xll.qlFuturesRateHelper(,$G5,$C5,$F5,$I$3,$H5,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>obj_00394#0001</v>
+        <v>obj_0026f#0001</v>
       </c>
       <c r="J5" s="48" t="str">
         <f>_xll.ohRangeRetrieveError(I5)</f>
@@ -12355,7 +12353,7 @@
       </c>
       <c r="I6" s="134" t="str">
         <f>_xll.qlFuturesRateHelper(,$G6,$C6,$F6,$I$3,$H6,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>obj_0038d#0001</v>
+        <v>obj_00274#0001</v>
       </c>
       <c r="J6" s="48" t="str">
         <f>_xll.ohRangeRetrieveError(I6)</f>
@@ -12391,7 +12389,7 @@
       </c>
       <c r="I7" s="134" t="str">
         <f>_xll.qlFuturesRateHelper(,$G7,$C7,$F7,$I$3,$H7,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>obj_00386#0001</v>
+        <v>obj_00277#0001</v>
       </c>
       <c r="J7" s="48" t="str">
         <f>_xll.ohRangeRetrieveError(I7)</f>
@@ -12427,7 +12425,7 @@
       </c>
       <c r="I8" s="134" t="str">
         <f>_xll.qlFuturesRateHelper(,$G8,$C8,$F8,$I$3,$H8,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>obj_00385#0001</v>
+        <v>obj_00273#0001</v>
       </c>
       <c r="J8" s="48" t="str">
         <f>_xll.ohRangeRetrieveError(I8)</f>
@@ -12463,7 +12461,7 @@
       </c>
       <c r="I9" s="134" t="str">
         <f>_xll.qlFuturesRateHelper(,$G9,$C9,$F9,$I$3,$H9,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>obj_00388#0001</v>
+        <v>obj_0027f#0001</v>
       </c>
       <c r="J9" s="48" t="str">
         <f>_xll.ohRangeRetrieveError(I9)</f>
@@ -12499,7 +12497,7 @@
       </c>
       <c r="I10" s="134" t="str">
         <f>_xll.qlFuturesRateHelper(,$G10,$C10,$F10,$I$3,$H10,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>obj_003a3#0001</v>
+        <v>obj_0026b#0001</v>
       </c>
       <c r="J10" s="48" t="str">
         <f>_xll.ohRangeRetrieveError(I10)</f>
@@ -12535,7 +12533,7 @@
       </c>
       <c r="I11" s="134" t="str">
         <f>_xll.qlFuturesRateHelper(,$G11,$C11,$F11,$I$3,$H11,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>obj_00397#0001</v>
+        <v>obj_00283#0001</v>
       </c>
       <c r="J11" s="48" t="str">
         <f>_xll.ohRangeRetrieveError(I11)</f>
@@ -12571,7 +12569,7 @@
       </c>
       <c r="I12" s="134" t="str">
         <f>_xll.qlFuturesRateHelper(,$G12,$C12,$F12,$I$3,$H12,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>obj_00393#0001</v>
+        <v>obj_00269#0001</v>
       </c>
       <c r="J12" s="48" t="str">
         <f>_xll.ohRangeRetrieveError(I12)</f>
@@ -12608,7 +12606,7 @@
       </c>
       <c r="I13" s="134" t="str">
         <f>_xll.qlFuturesRateHelper(,$G13,$C13,$F13,$I$3,$H13,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>obj_00390#0001</v>
+        <v>obj_00284#0001</v>
       </c>
       <c r="J13" s="48" t="str">
         <f>_xll.ohRangeRetrieveError(I13)</f>
@@ -12645,7 +12643,7 @@
       </c>
       <c r="I14" s="134" t="str">
         <f>_xll.qlFuturesRateHelper(,$G14,$C14,$F14,$I$3,$H14,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>obj_0039f#0001</v>
+        <v>obj_0027d#0001</v>
       </c>
       <c r="J14" s="48" t="str">
         <f>_xll.ohRangeRetrieveError(I14)</f>
@@ -12682,7 +12680,7 @@
       </c>
       <c r="I15" s="134" t="str">
         <f>_xll.qlFuturesRateHelper(,$G15,$C15,$F15,$I$3,$H15,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>obj_00380#0001</v>
+        <v>obj_0027e#0001</v>
       </c>
       <c r="J15" s="48" t="str">
         <f>_xll.ohRangeRetrieveError(I15)</f>
@@ -12719,7 +12717,7 @@
       </c>
       <c r="I16" s="134" t="str">
         <f>_xll.qlFuturesRateHelper(,$G16,$C16,$F16,$I$3,$H16,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>obj_0037e#0001</v>
+        <v>obj_00281#0001</v>
       </c>
       <c r="J16" s="48" t="str">
         <f>_xll.ohRangeRetrieveError(I16)</f>
@@ -12756,7 +12754,7 @@
       </c>
       <c r="I17" s="134" t="str">
         <f>_xll.qlFuturesRateHelper(,$G17,$C17,$F17,$I$3,$H17,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>obj_00392#0001</v>
+        <v>obj_00263#0001</v>
       </c>
       <c r="J17" s="48" t="str">
         <f>_xll.ohRangeRetrieveError(I17)</f>
@@ -12793,7 +12791,7 @@
       </c>
       <c r="I18" s="134" t="str">
         <f>_xll.qlFuturesRateHelper(,$G18,$C18,$F18,$I$3,$H18,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>obj_0038f#0001</v>
+        <v>obj_0027c#0001</v>
       </c>
       <c r="J18" s="48" t="str">
         <f>_xll.ohRangeRetrieveError(I18)</f>
@@ -12830,7 +12828,7 @@
       </c>
       <c r="I19" s="134" t="str">
         <f>_xll.qlFuturesRateHelper(,$G19,$C19,$F19,$I$3,$H19,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>obj_0038e#0001</v>
+        <v>obj_00278#0001</v>
       </c>
       <c r="J19" s="48" t="str">
         <f>_xll.ohRangeRetrieveError(I19)</f>
@@ -12867,7 +12865,7 @@
       </c>
       <c r="I20" s="134" t="str">
         <f>_xll.qlFuturesRateHelper(,$G20,$C20,$F20,$I$3,$H20,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>obj_003a0#0001</v>
+        <v>obj_00285#0001</v>
       </c>
       <c r="J20" s="48" t="str">
         <f>_xll.ohRangeRetrieveError(I20)</f>
@@ -12904,7 +12902,7 @@
       </c>
       <c r="I21" s="134" t="str">
         <f>_xll.qlFuturesRateHelper(,$G21,$C21,$F21,$I$3,$H21,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>obj_0039d#0001</v>
+        <v>obj_00276#0001</v>
       </c>
       <c r="J21" s="48" t="str">
         <f>_xll.ohRangeRetrieveError(I21)</f>
@@ -12941,7 +12939,7 @@
       </c>
       <c r="I22" s="134" t="str">
         <f>_xll.qlFuturesRateHelper(,$G22,$C22,$F22,$I$3,$H22,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>obj_00383#0001</v>
+        <v>obj_00267#0001</v>
       </c>
       <c r="J22" s="48" t="str">
         <f>_xll.ohRangeRetrieveError(I22)</f>
@@ -12978,7 +12976,7 @@
       </c>
       <c r="I23" s="134" t="str">
         <f>_xll.qlFuturesRateHelper(,$G23,$C23,$F23,$I$3,$H23,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>obj_00396#0001</v>
+        <v>obj_00279#0001</v>
       </c>
       <c r="J23" s="48" t="str">
         <f>_xll.ohRangeRetrieveError(I23)</f>
@@ -13015,7 +13013,7 @@
       </c>
       <c r="I24" s="134" t="str">
         <f>_xll.qlFuturesRateHelper(,$G24,$C24,$F24,$I$3,$H24,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>obj_0037f#0001</v>
+        <v>obj_00282#0001</v>
       </c>
       <c r="J24" s="48" t="str">
         <f>_xll.ohRangeRetrieveError(I24)</f>
@@ -13052,7 +13050,7 @@
       </c>
       <c r="I25" s="134" t="str">
         <f>_xll.qlFuturesRateHelper(,$G25,$C25,$F25,$I$3,$H25,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>obj_0039e#0001</v>
+        <v>obj_0027a#0001</v>
       </c>
       <c r="J25" s="48" t="str">
         <f>_xll.ohRangeRetrieveError(I25)</f>
@@ -13089,7 +13087,7 @@
       </c>
       <c r="I26" s="134" t="str">
         <f>_xll.qlFuturesRateHelper(,$G26,$C26,$F26,$I$3,$H26,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>obj_0039a#0001</v>
+        <v>obj_00264#0001</v>
       </c>
       <c r="J26" s="48" t="str">
         <f>_xll.ohRangeRetrieveError(I26)</f>
@@ -13126,7 +13124,7 @@
       </c>
       <c r="I27" s="134" t="str">
         <f>_xll.qlFuturesRateHelper(,$G27,$C27,$F27,$I$3,$H27,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>obj_00382#0001</v>
+        <v>obj_00261#0001</v>
       </c>
       <c r="J27" s="48" t="str">
         <f>_xll.ohRangeRetrieveError(I27)</f>
@@ -13163,7 +13161,7 @@
       </c>
       <c r="I28" s="134" t="str">
         <f>_xll.qlFuturesRateHelper(,$G28,$C28,$F28,$I$3,$H28,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>obj_00389#0001</v>
+        <v>obj_0025d#0001</v>
       </c>
       <c r="J28" s="48" t="str">
         <f>_xll.ohRangeRetrieveError(I28)</f>
@@ -13200,7 +13198,7 @@
       </c>
       <c r="I29" s="134" t="str">
         <f>_xll.qlFuturesRateHelper(,$G29,$C29,$F29,$I$3,$H29,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>obj_003a2#0001</v>
+        <v>obj_00265#0001</v>
       </c>
       <c r="J29" s="48" t="str">
         <f>_xll.ohRangeRetrieveError(I29)</f>
@@ -13237,7 +13235,7 @@
       </c>
       <c r="I30" s="134" t="str">
         <f>_xll.qlFuturesRateHelper(,$G30,$C30,$F30,$I$3,$H30,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>obj_0039c#0001</v>
+        <v>obj_00270#0001</v>
       </c>
       <c r="J30" s="48" t="str">
         <f>_xll.ohRangeRetrieveError(I30)</f>
@@ -13274,7 +13272,7 @@
       </c>
       <c r="I31" s="134" t="str">
         <f>_xll.qlFuturesRateHelper(,$G31,$C31,$F31,$I$3,$H31,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>obj_0037b#0001</v>
+        <v>obj_00266#0001</v>
       </c>
       <c r="J31" s="48" t="str">
         <f>_xll.ohRangeRetrieveError(I31)</f>
@@ -13311,7 +13309,7 @@
       </c>
       <c r="I32" s="134" t="str">
         <f>_xll.qlFuturesRateHelper(,$G32,$C32,$F32,$I$3,$H32,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>obj_0038a#0001</v>
+        <v>obj_00262#0001</v>
       </c>
       <c r="J32" s="48" t="str">
         <f>_xll.ohRangeRetrieveError(I32)</f>
@@ -13348,7 +13346,7 @@
       </c>
       <c r="I33" s="134" t="str">
         <f>_xll.qlFuturesRateHelper(,$G33,$C33,$F33,$I$3,$H33,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>obj_0038c#0001</v>
+        <v>obj_0026e#0001</v>
       </c>
       <c r="J33" s="48" t="str">
         <f>_xll.ohRangeRetrieveError(I33)</f>
@@ -13385,7 +13383,7 @@
       </c>
       <c r="I34" s="134" t="str">
         <f>_xll.qlFuturesRateHelper(,$G34,$C34,$F34,$I$3,$H34,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>obj_0037d#0001</v>
+        <v>obj_00272#0001</v>
       </c>
       <c r="J34" s="48" t="str">
         <f>_xll.ohRangeRetrieveError(I34)</f>
@@ -13422,7 +13420,7 @@
       </c>
       <c r="I35" s="134" t="str">
         <f>_xll.qlFuturesRateHelper(,$G35,$C35,$F35,$I$3,$H35,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>obj_00398#0001</v>
+        <v>obj_00280#0001</v>
       </c>
       <c r="J35" s="48" t="str">
         <f>_xll.ohRangeRetrieveError(I35)</f>
@@ -13459,7 +13457,7 @@
       </c>
       <c r="I36" s="134" t="str">
         <f>_xll.qlFuturesRateHelper(,$G36,$C36,$F36,$I$3,$H36,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>obj_0037c#0001</v>
+        <v>obj_0026c#0001</v>
       </c>
       <c r="J36" s="48" t="str">
         <f>_xll.ohRangeRetrieveError(I36)</f>
@@ -13496,7 +13494,7 @@
       </c>
       <c r="I37" s="134" t="str">
         <f>_xll.qlFuturesRateHelper(,$G37,$C37,$F37,$I$3,$H37,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>obj_003a4#0001</v>
+        <v>obj_00271#0001</v>
       </c>
       <c r="J37" s="48" t="str">
         <f>_xll.ohRangeRetrieveError(I37)</f>
@@ -13533,7 +13531,7 @@
       </c>
       <c r="I38" s="134" t="str">
         <f>_xll.qlFuturesRateHelper(,$G38,$C38,$F38,$I$3,$H38,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>obj_00391#0001</v>
+        <v>obj_0025e#0001</v>
       </c>
       <c r="J38" s="48" t="str">
         <f>_xll.ohRangeRetrieveError(I38)</f>
@@ -13570,7 +13568,7 @@
       </c>
       <c r="I39" s="134" t="str">
         <f>_xll.qlFuturesRateHelper(,$G39,$C39,$F39,$I$3,$H39,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>obj_0038b#0001</v>
+        <v>obj_00268#0001</v>
       </c>
       <c r="J39" s="48" t="str">
         <f>_xll.ohRangeRetrieveError(I39)</f>
@@ -13607,7 +13605,7 @@
       </c>
       <c r="I40" s="134" t="str">
         <f>_xll.qlFuturesRateHelper(,$G40,$C40,$F40,$I$3,$H40,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>obj_00387#0001</v>
+        <v>obj_0027b#0001</v>
       </c>
       <c r="J40" s="48" t="str">
         <f>_xll.ohRangeRetrieveError(I40)</f>
@@ -13644,7 +13642,7 @@
       </c>
       <c r="I41" s="134" t="str">
         <f>_xll.qlFuturesRateHelper(,$G41,$C41,$F41,$I$3,$H41,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>obj_0039b#0001</v>
+        <v>obj_0026a#0001</v>
       </c>
       <c r="J41" s="48" t="str">
         <f>_xll.ohRangeRetrieveError(I41)</f>
@@ -13681,7 +13679,7 @@
       </c>
       <c r="I42" s="134" t="str">
         <f>_xll.qlFuturesRateHelper(,$G42,$C42,$F42,$I$3,$H42,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>obj_00395#0001</v>
+        <v>obj_00275#0001</v>
       </c>
       <c r="J42" s="48" t="str">
         <f>_xll.ohRangeRetrieveError(I42)</f>
@@ -13717,7 +13715,7 @@
       </c>
       <c r="I43" s="134" t="str">
         <f>_xll.qlFuturesRateHelper(,$G43,$C43,$F43,$I$3,$H43,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>obj_003a1#0001</v>
+        <v>obj_00260#0001</v>
       </c>
       <c r="J43" s="48" t="str">
         <f>_xll.ohRangeRetrieveError(I43)</f>
@@ -13753,7 +13751,7 @@
       </c>
       <c r="I44" s="134" t="str">
         <f>_xll.qlFuturesRateHelper(,$G44,$C44,$F44,$I$3,$H44,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>obj_00381#0001</v>
+        <v>obj_0025c#0001</v>
       </c>
       <c r="J44" s="48" t="str">
         <f>_xll.ohRangeRetrieveError(I44)</f>
@@ -13789,7 +13787,7 @@
       </c>
       <c r="I45" s="134" t="str">
         <f>_xll.qlFuturesRateHelper(,$G45,$C45,$F45,$I$3,$H45,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>obj_00384#0001</v>
+        <v>obj_0026d#0001</v>
       </c>
       <c r="J45" s="48" t="str">
         <f>_xll.ohRangeRetrieveError(I45)</f>
@@ -13825,7 +13823,7 @@
       </c>
       <c r="I46" s="134" t="str">
         <f>_xll.qlFuturesRateHelper(,$G46,$C46,$F46,$I$3,$H46,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>obj_00399#0001</v>
+        <v>obj_0025f#0001</v>
       </c>
       <c r="J46" s="48" t="str">
         <f>_xll.ohRangeRetrieveError(I46)</f>
@@ -13962,7 +13960,7 @@
       <c r="K3" s="63"/>
       <c r="L3" s="160" t="str">
         <f>_xll.qlIborIndex(,FamilyName,IndexTenor,NDays,Currency,Calendar,"mf",TRUE,"Actual/365 (fixed)",,,Trigger,ObjectOverwrite)</f>
-        <v>obj_0025e#0003</v>
+        <v>obj_0029a#0001</v>
       </c>
       <c r="M3" s="141" t="str">
         <f>_xll.ohRangeRetrieveError(L3)</f>
@@ -13984,7 +13982,7 @@
       <c r="K4" s="63"/>
       <c r="L4" s="161" t="str">
         <f>_xll.qlIborIndex(,FamilyName,"6M",NDays,Currency,Calendar,"mf",TRUE,"Actual/365 (fixed)",,,Trigger,ObjectOverwrite)</f>
-        <v>obj_0024f#0003</v>
+        <v>obj_00298#0001</v>
       </c>
       <c r="M4" s="141" t="str">
         <f>_xll.ohRangeRetrieveError(L4)</f>
@@ -14046,7 +14044,7 @@
       </c>
       <c r="L6" s="157" t="str">
         <f>_xll.qlSwapRateHelper2(,$K6,B6,$D6,Calendar,$G6,$H6,$I6,$L$3,$J6,C6,,Permanent,,ObjectOverwrite)</f>
-        <v>obj_003a5#0015</v>
+        <v>obj_002be#0001</v>
       </c>
       <c r="M6" s="139" t="str">
         <f>_xll.ohRangeRetrieveError(L6)</f>
@@ -14092,7 +14090,7 @@
       </c>
       <c r="L7" s="157" t="str">
         <f>_xll.qlSwapRateHelper2(,$K7,B7,$D7,Calendar,$G7,$H7,$I7,$L$3,$J7,C7,,Permanent,,ObjectOverwrite)</f>
-        <v>obj_003a6#0000</v>
+        <v>obj_002bd#0001</v>
       </c>
       <c r="M7" s="139" t="str">
         <f>_xll.ohRangeRetrieveError(L7)</f>
@@ -14138,7 +14136,7 @@
       </c>
       <c r="L8" s="157" t="str">
         <f>_xll.qlSwapRateHelper2(,$K8,B8,$D8,Calendar,$G8,$H8,$I8,$L$3,$J8,C8,,Permanent,,ObjectOverwrite)</f>
-        <v>obj_003a7#0000</v>
+        <v>obj_002bc#0001</v>
       </c>
       <c r="M8" s="139" t="str">
         <f>_xll.ohRangeRetrieveError(L8)</f>
@@ -14184,7 +14182,7 @@
       </c>
       <c r="L9" s="157" t="str">
         <f>_xll.qlSwapRateHelper2(,$K9,B9,$D9,Calendar,$G9,$H9,$I9,$L$3,$J9,C9,,Permanent,,ObjectOverwrite)</f>
-        <v>obj_003a8#0000</v>
+        <v>obj_002bb#0001</v>
       </c>
       <c r="M9" s="139" t="str">
         <f>_xll.ohRangeRetrieveError(L9)</f>
@@ -14230,7 +14228,7 @@
       </c>
       <c r="L10" s="157" t="str">
         <f>_xll.qlSwapRateHelper2(,$K10,B10,$D10,Calendar,$G10,$H10,$I10,$L$3,$J10,C10,,Permanent,,ObjectOverwrite)</f>
-        <v>obj_003aa#0000</v>
+        <v>obj_002bf#0001</v>
       </c>
       <c r="M10" s="139" t="str">
         <f>_xll.ohRangeRetrieveError(L10)</f>
@@ -14276,7 +14274,7 @@
       </c>
       <c r="L11" s="157" t="str">
         <f>_xll.qlSwapRateHelper2(,$K11,B11,$D11,Calendar,$G11,$H11,$I11,$L$3,$J11,C11,,Permanent,,ObjectOverwrite)</f>
-        <v>obj_003a9#0000</v>
+        <v>obj_002ba#0001</v>
       </c>
       <c r="M11" s="139" t="str">
         <f>_xll.ohRangeRetrieveError(L11)</f>
@@ -14322,7 +14320,7 @@
       </c>
       <c r="L12" s="144" t="str">
         <f>_xll.qlSwapRateHelper2(,$K12,B12,$D12,Calendar,$G12,$H12,$I12,$L$4,$J12,C12,,Permanent,,ObjectOverwrite)</f>
-        <v>obj_003ab#0013</v>
+        <v>obj_002aa#0001</v>
       </c>
       <c r="M12" s="139" t="str">
         <f>_xll.ohRangeRetrieveError(L12)</f>
@@ -14367,7 +14365,7 @@
       </c>
       <c r="L13" s="144" t="str">
         <f>_xll.qlSwapRateHelper2(,$K13,B13,$D13,Calendar,$G13,$H13,$I13,$L$4,$J13,C13,,Permanent,,ObjectOverwrite)</f>
-        <v>obj_003ac#0000</v>
+        <v>obj_002a6#0001</v>
       </c>
       <c r="M13" s="139" t="str">
         <f>_xll.ohRangeRetrieveError(L13)</f>
@@ -14412,7 +14410,7 @@
       </c>
       <c r="L14" s="144" t="str">
         <f>_xll.qlSwapRateHelper2(,$K14,B14,$D14,Calendar,$G14,$H14,$I14,$L$4,$J14,C14,,Permanent,,ObjectOverwrite)</f>
-        <v>obj_003b3#0000</v>
+        <v>obj_002a9#0001</v>
       </c>
       <c r="M14" s="139" t="str">
         <f>_xll.ohRangeRetrieveError(L14)</f>
@@ -14456,7 +14454,7 @@
       </c>
       <c r="L15" s="144" t="str">
         <f>_xll.qlSwapRateHelper2(,$K15,B15,$D15,Calendar,$G15,$H15,$I15,$L$4,$J15,C15,,Permanent,,ObjectOverwrite)</f>
-        <v>obj_003b9#0000</v>
+        <v>obj_002b0#0001</v>
       </c>
       <c r="M15" s="139" t="str">
         <f>_xll.ohRangeRetrieveError(L15)</f>
@@ -14500,7 +14498,7 @@
       </c>
       <c r="L16" s="144" t="str">
         <f>_xll.qlSwapRateHelper2(,$K16,B16,$D16,Calendar,$G16,$H16,$I16,$L$4,$J16,C16,,Permanent,,ObjectOverwrite)</f>
-        <v>obj_003bb#0000</v>
+        <v>obj_002a8#0001</v>
       </c>
       <c r="M16" s="139" t="str">
         <f>_xll.ohRangeRetrieveError(L16)</f>
@@ -14544,7 +14542,7 @@
       </c>
       <c r="L17" s="144" t="str">
         <f>_xll.qlSwapRateHelper2(,$K17,B17,$D17,Calendar,$G17,$H17,$I17,$L$4,$J17,C17,,Permanent,,ObjectOverwrite)</f>
-        <v>obj_003bd#0000</v>
+        <v>obj_002a1#0001</v>
       </c>
       <c r="M17" s="139" t="str">
         <f>_xll.ohRangeRetrieveError(L17)</f>
@@ -14588,7 +14586,7 @@
       </c>
       <c r="L18" s="144" t="str">
         <f>_xll.qlSwapRateHelper2(,$K18,B18,$D18,Calendar,$G18,$H18,$I18,$L$4,$J18,C18,,Permanent,,ObjectOverwrite)</f>
-        <v>obj_003c0#0000</v>
+        <v>obj_002b3#0001</v>
       </c>
       <c r="M18" s="139" t="str">
         <f>_xll.ohRangeRetrieveError(L18)</f>
@@ -14632,7 +14630,7 @@
       </c>
       <c r="L19" s="144" t="str">
         <f>_xll.qlSwapRateHelper2(,$K19,B19,$D19,Calendar,$G19,$H19,$I19,$L$4,$J19,C19,,Permanent,,ObjectOverwrite)</f>
-        <v>obj_003c3#0000</v>
+        <v>obj_002a7#0001</v>
       </c>
       <c r="M19" s="139" t="str">
         <f>_xll.ohRangeRetrieveError(L19)</f>
@@ -14675,7 +14673,7 @@
       </c>
       <c r="L20" s="144" t="str">
         <f>_xll.qlSwapRateHelper2(,$K20,B20,$D20,Calendar,$G20,$H20,$I20,$L$4,$J20,C20,,Permanent,,ObjectOverwrite)</f>
-        <v>obj_003c6#0000</v>
+        <v>obj_0029b#0001</v>
       </c>
       <c r="M20" s="139" t="str">
         <f>_xll.ohRangeRetrieveError(L20)</f>
@@ -14718,7 +14716,7 @@
       </c>
       <c r="L21" s="144" t="str">
         <f>_xll.qlSwapRateHelper2(,$K21,B21,$D21,Calendar,$G21,$H21,$I21,$L$4,$J21,C21,,Permanent,,ObjectOverwrite)</f>
-        <v>obj_003ad#0000</v>
+        <v>obj_002a2#0001</v>
       </c>
       <c r="M21" s="139" t="str">
         <f>_xll.ohRangeRetrieveError(L21)</f>
@@ -14761,7 +14759,7 @@
       </c>
       <c r="L22" s="144" t="str">
         <f>_xll.qlSwapRateHelper2(,$K22,B22,$D22,Calendar,$G22,$H22,$I22,$L$4,$J22,C22,,Permanent,,ObjectOverwrite)</f>
-        <v>obj_003b4#0000</v>
+        <v>obj_002a5#0001</v>
       </c>
       <c r="M22" s="139" t="str">
         <f>_xll.ohRangeRetrieveError(L22)</f>
@@ -14804,7 +14802,7 @@
       </c>
       <c r="L23" s="144" t="str">
         <f>_xll.qlSwapRateHelper2(,$K23,B23,$D23,Calendar,$G23,$H23,$I23,$L$4,$J23,C23,,Permanent,,ObjectOverwrite)</f>
-        <v>obj_003b0#0000</v>
+        <v>obj_002b5#0001</v>
       </c>
       <c r="M23" s="139" t="str">
         <f>_xll.ohRangeRetrieveError(L23)</f>
@@ -14847,7 +14845,7 @@
       </c>
       <c r="L24" s="144" t="str">
         <f>_xll.qlSwapRateHelper2(,$K24,B24,$D24,Calendar,$G24,$H24,$I24,$L$4,$J24,C24,,Permanent,,ObjectOverwrite)</f>
-        <v>obj_003bc#0000</v>
+        <v>obj_002a4#0001</v>
       </c>
       <c r="M24" s="139" t="str">
         <f>_xll.ohRangeRetrieveError(L24)</f>
@@ -14890,7 +14888,7 @@
       </c>
       <c r="L25" s="144" t="str">
         <f>_xll.qlSwapRateHelper2(,$K25,B25,$D25,Calendar,$G25,$H25,$I25,$L$4,$J25,C25,,Permanent,,ObjectOverwrite)</f>
-        <v>obj_003be#0000</v>
+        <v>obj_0029e#0001</v>
       </c>
       <c r="M25" s="139" t="str">
         <f>_xll.ohRangeRetrieveError(L25)</f>
@@ -14933,7 +14931,7 @@
       </c>
       <c r="L26" s="144" t="str">
         <f>_xll.qlSwapRateHelper2(,$K26,B26,$D26,Calendar,$G26,$H26,$I26,$L$4,$J26,C26,,Permanent,,ObjectOverwrite)</f>
-        <v>obj_003c1#0000</v>
+        <v>obj_002af#0001</v>
       </c>
       <c r="M26" s="139" t="str">
         <f>_xll.ohRangeRetrieveError(L26)</f>
@@ -14976,7 +14974,7 @@
       </c>
       <c r="L27" s="144" t="str">
         <f>_xll.qlSwapRateHelper2(,$K27,B27,$D27,Calendar,$G27,$H27,$I27,$L$4,$J27,C27,,Permanent,,ObjectOverwrite)</f>
-        <v>obj_003c4#0000</v>
+        <v>obj_002a3#0001</v>
       </c>
       <c r="M27" s="139" t="str">
         <f>_xll.ohRangeRetrieveError(L27)</f>
@@ -15019,7 +15017,7 @@
       </c>
       <c r="L28" s="144" t="str">
         <f>_xll.qlSwapRateHelper2(,$K28,B28,$D28,Calendar,$G28,$H28,$I28,$L$4,$J28,C28,,Permanent,,ObjectOverwrite)</f>
-        <v>obj_003c7#0000</v>
+        <v>obj_002b6#0001</v>
       </c>
       <c r="M28" s="139" t="str">
         <f>_xll.ohRangeRetrieveError(L28)</f>
@@ -15062,7 +15060,7 @@
       </c>
       <c r="L29" s="144" t="str">
         <f>_xll.qlSwapRateHelper2(,$K29,B29,$D29,Calendar,$G29,$H29,$I29,$L$4,$J29,C29,,Permanent,,ObjectOverwrite)</f>
-        <v>obj_003ae#0000</v>
+        <v>obj_0029f#0001</v>
       </c>
       <c r="M29" s="139" t="str">
         <f>_xll.ohRangeRetrieveError(L29)</f>
@@ -15105,7 +15103,7 @@
       </c>
       <c r="L30" s="144" t="str">
         <f>_xll.qlSwapRateHelper2(,$K30,B30,$D30,Calendar,$G30,$H30,$I30,$L$4,$J30,C30,,Permanent,,ObjectOverwrite)</f>
-        <v>obj_003b5#0000</v>
+        <v>obj_0029d#0001</v>
       </c>
       <c r="M30" s="139" t="str">
         <f>_xll.ohRangeRetrieveError(L30)</f>
@@ -15148,7 +15146,7 @@
       </c>
       <c r="L31" s="144" t="str">
         <f>_xll.qlSwapRateHelper2(,$K31,B31,$D31,Calendar,$G31,$H31,$I31,$L$4,$J31,C31,,Permanent,,ObjectOverwrite)</f>
-        <v>obj_003b7#0000</v>
+        <v>obj_002b8#0001</v>
       </c>
       <c r="M31" s="139" t="str">
         <f>_xll.ohRangeRetrieveError(L31)</f>
@@ -15191,7 +15189,7 @@
       </c>
       <c r="L32" s="144" t="str">
         <f>_xll.qlSwapRateHelper2(,$K32,B32,$D32,Calendar,$G32,$H32,$I32,$L$4,$J32,C32,,Permanent,,ObjectOverwrite)</f>
-        <v>obj_003b8#0000</v>
+        <v>obj_002b4#0001</v>
       </c>
       <c r="M32" s="139" t="str">
         <f>_xll.ohRangeRetrieveError(L32)</f>
@@ -15234,7 +15232,7 @@
       </c>
       <c r="L33" s="144" t="str">
         <f>_xll.qlSwapRateHelper2(,$K33,B33,$D33,Calendar,$G33,$H33,$I33,$L$4,$J33,C33,,Permanent,,ObjectOverwrite)</f>
-        <v>obj_003b2#0000</v>
+        <v>obj_002ad#0001</v>
       </c>
       <c r="M33" s="139" t="str">
         <f>_xll.ohRangeRetrieveError(L33)</f>
@@ -15277,7 +15275,7 @@
       </c>
       <c r="L34" s="144" t="str">
         <f>_xll.qlSwapRateHelper2(,$K34,B34,$D34,Calendar,$G34,$H34,$I34,$L$4,$J34,C34,,Permanent,,ObjectOverwrite)</f>
-        <v>obj_003c2#0000</v>
+        <v>obj_002ab#0001</v>
       </c>
       <c r="M34" s="139" t="str">
         <f>_xll.ohRangeRetrieveError(L34)</f>
@@ -15320,7 +15318,7 @@
       </c>
       <c r="L35" s="144" t="str">
         <f>_xll.qlSwapRateHelper2(,$K35,B35,$D35,Calendar,$G35,$H35,$I35,$L$4,$J35,C35,,Permanent,,ObjectOverwrite)</f>
-        <v>obj_003c5#0000</v>
+        <v>obj_002a0#0001</v>
       </c>
       <c r="M35" s="139" t="str">
         <f>_xll.ohRangeRetrieveError(L35)</f>
@@ -15363,7 +15361,7 @@
       </c>
       <c r="L36" s="144" t="str">
         <f>_xll.qlSwapRateHelper2(,$K36,B36,$D36,Calendar,$G36,$H36,$I36,$L$4,$J36,C36,,Permanent,,ObjectOverwrite)</f>
-        <v>obj_003c8#0000</v>
+        <v>obj_002b2#0001</v>
       </c>
       <c r="M36" s="139" t="str">
         <f>_xll.ohRangeRetrieveError(L36)</f>
@@ -15406,7 +15404,7 @@
       </c>
       <c r="L37" s="144" t="str">
         <f>_xll.qlSwapRateHelper2(,$K37,B37,$D37,Calendar,$G37,$H37,$I37,$L$4,$J37,C37,,Permanent,,ObjectOverwrite)</f>
-        <v>obj_003af#0000</v>
+        <v>obj_002b9#0001</v>
       </c>
       <c r="M37" s="139" t="str">
         <f>_xll.ohRangeRetrieveError(L37)</f>
@@ -15449,7 +15447,7 @@
       </c>
       <c r="L38" s="144" t="str">
         <f>_xll.qlSwapRateHelper2(,$K38,B38,$D38,Calendar,$G38,$H38,$I38,$L$4,$J38,C38,,Permanent,,ObjectOverwrite)</f>
-        <v>obj_003b6#0000</v>
+        <v>obj_0029c#0001</v>
       </c>
       <c r="M38" s="139" t="str">
         <f>_xll.ohRangeRetrieveError(L38)</f>
@@ -15492,7 +15490,7 @@
       </c>
       <c r="L39" s="144" t="str">
         <f>_xll.qlSwapRateHelper2(,$K39,B39,$D39,Calendar,$G39,$H39,$I39,$L$4,$J39,C39,,Permanent,,ObjectOverwrite)</f>
-        <v>obj_003b1#0000</v>
+        <v>obj_002b1#0001</v>
       </c>
       <c r="M39" s="139" t="str">
         <f>_xll.ohRangeRetrieveError(L39)</f>
@@ -15535,7 +15533,7 @@
       </c>
       <c r="L40" s="144" t="str">
         <f>_xll.qlSwapRateHelper2(,$K40,B40,$D40,Calendar,$G40,$H40,$I40,$L$4,$J40,C40,,Permanent,,ObjectOverwrite)</f>
-        <v>obj_003ba#0000</v>
+        <v>obj_002ac#0001</v>
       </c>
       <c r="M40" s="139" t="str">
         <f>_xll.ohRangeRetrieveError(L40)</f>
@@ -15578,7 +15576,7 @@
       </c>
       <c r="L41" s="144" t="str">
         <f>_xll.qlSwapRateHelper2(,$K41,B41,$D41,Calendar,$G41,$H41,$I41,$L$4,$J41,C41,,Permanent,,ObjectOverwrite)</f>
-        <v>obj_003bf#0000</v>
+        <v>obj_002b7#0001</v>
       </c>
       <c r="M41" s="139" t="str">
         <f>_xll.ohRangeRetrieveError(L41)</f>
@@ -15621,7 +15619,7 @@
       </c>
       <c r="L42" s="144" t="str">
         <f>_xll.qlSwapRateHelper2(,$K42,B42,$D42,Calendar,$G42,$H42,$I42,$L$4,$J42,C42,,Permanent,,ObjectOverwrite)</f>
-        <v>obj_003c9#0000</v>
+        <v>obj_002ae#0001</v>
       </c>
       <c r="M42" s="139" t="str">
         <f>_xll.ohRangeRetrieveError(L42)</f>

</xml_diff>